<commit_message>
New files to the folders
</commit_message>
<xml_diff>
--- a/iApply_CCBS_Interfaces.xlsx
+++ b/iApply_CCBS_Interfaces.xlsx
@@ -1,34 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20401"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB9AD2B-FB38-4313-8576-7D8E37A6610F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E05BC8-8E72-48FA-8B5C-9489B2929E91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9390" windowWidth="29040" windowHeight="16440" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11025" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CCBS_API_CALLS" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="325">
   <si>
     <t>INSERT</t>
   </si>
@@ -1009,6 +996,21 @@
   </si>
   <si>
     <t>03. RepaymentSchedule</t>
+  </si>
+  <si>
+    <t>CollateralMaintenance_Finalize.xlsx</t>
+  </si>
+  <si>
+    <t>CollateralMaintenance_Create.xlsx</t>
+  </si>
+  <si>
+    <t>CollateralMaintenance_CreateFinalize.xlsx</t>
+  </si>
+  <si>
+    <t>CollateralMaintenance_Update.xlsx</t>
+  </si>
+  <si>
+    <t>DepositAccountOpening.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1194,6 +1196,20 @@
   <dxfs count="17">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1205,20 +1221,6 @@
         <vertAlign val="baseline"/>
         <sz val="9"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1476,7 +1478,7 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:P93">
+  <sortState ref="B3:P93">
     <sortCondition ref="F3:F99"/>
     <sortCondition ref="G3:G99"/>
     <sortCondition ref="C3:C99"/>
@@ -1495,17 +1497,17 @@
     <tableColumn id="10" xr3:uid="{1001738D-9F43-4460-B2E4-6382DE0B68F5}" name="Commands" dataDxfId="4"/>
     <tableColumn id="9" xr3:uid="{F1FE272B-50F9-4D94-A2AD-ABFD6BB3EA40}" name="Excel File Names" dataDxfId="3"/>
     <tableColumn id="12" xr3:uid="{924387FC-EFCA-4D58-8137-D53D3D025A51}" name="Depreciated Excel Files" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{BA600521-ABEF-4B3F-A98A-CC6AC4090B06}" name="IntFileNum" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{D32DAD5E-1164-4F66-90AE-2CFBD99C59B0}" name="C1" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{BA600521-ABEF-4B3F-A98A-CC6AC4090B06}" name="IntFileNum" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{D32DAD5E-1164-4F66-90AE-2CFBD99C59B0}" name="C1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1543,9 +1545,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1578,9 +1580,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1613,9 +1632,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1794,37 +1830,37 @@
   </sheetPr>
   <dimension ref="B1:T100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.5546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.21875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="8.88671875" style="2"/>
-    <col min="18" max="18" width="14.44140625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" style="2"/>
-    <col min="20" max="20" width="14.44140625" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="8.88671875" style="2"/>
+    <col min="14" max="14" width="35.5703125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" style="2"/>
+    <col min="18" max="18" width="14.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" style="2"/>
+    <col min="20" max="20" width="14.42578125" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="8.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
       <c r="C1" s="17">
         <v>3</v>
@@ -1843,7 +1879,7 @@
       <c r="M1" s="3"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="2:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>272</v>
       </c>
@@ -1890,7 +1926,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="48" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" ht="60" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>269</v>
       </c>
@@ -1929,7 +1965,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>269</v>
       </c>
@@ -1968,7 +2004,7 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="2:16" ht="36" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>269</v>
       </c>
@@ -2011,7 +2047,7 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>270</v>
       </c>
@@ -2046,7 +2082,7 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="2:16" ht="48" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" ht="48" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>269</v>
       </c>
@@ -2089,7 +2125,7 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="2:16" ht="48" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" ht="48" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
         <v>269</v>
       </c>
@@ -2132,7 +2168,7 @@
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="2:16" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>269</v>
       </c>
@@ -2171,7 +2207,7 @@
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>269</v>
       </c>
@@ -2208,7 +2244,7 @@
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>269</v>
       </c>
@@ -2247,7 +2283,7 @@
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>269</v>
       </c>
@@ -2284,7 +2320,7 @@
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>270</v>
       </c>
@@ -2317,7 +2353,7 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
         <v>269</v>
       </c>
@@ -2358,7 +2394,7 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
         <v>270</v>
       </c>
@@ -2391,7 +2427,7 @@
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="2:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
         <v>269</v>
       </c>
@@ -2430,7 +2466,7 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="2:16" ht="36" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
         <v>269</v>
       </c>
@@ -2471,7 +2507,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" s="9" t="s">
         <v>271</v>
       </c>
@@ -2502,7 +2538,7 @@
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
-    <row r="19" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B19" s="9" t="s">
         <v>271</v>
       </c>
@@ -2533,7 +2569,7 @@
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
     </row>
-    <row r="20" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" s="9" t="s">
         <v>271</v>
       </c>
@@ -2564,7 +2600,7 @@
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B21" s="9" t="s">
         <v>271</v>
       </c>
@@ -2595,7 +2631,7 @@
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
     </row>
-    <row r="22" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" s="9" t="s">
         <v>271</v>
       </c>
@@ -2626,7 +2662,7 @@
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" s="9" t="s">
         <v>271</v>
       </c>
@@ -2657,7 +2693,7 @@
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B24" s="9" t="s">
         <v>271</v>
       </c>
@@ -2688,7 +2724,7 @@
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
         <v>271</v>
       </c>
@@ -2719,7 +2755,7 @@
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" s="9" t="s">
         <v>271</v>
       </c>
@@ -2750,7 +2786,7 @@
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B27" s="9" t="s">
         <v>271</v>
       </c>
@@ -2781,7 +2817,7 @@
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
     </row>
-    <row r="28" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" s="9" t="s">
         <v>271</v>
       </c>
@@ -2812,7 +2848,7 @@
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
     </row>
-    <row r="29" spans="2:16" ht="36" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" ht="48" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
         <v>269</v>
       </c>
@@ -2853,7 +2889,7 @@
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
     </row>
-    <row r="30" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
         <v>269</v>
       </c>
@@ -2890,7 +2926,7 @@
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
     </row>
-    <row r="31" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
         <v>269</v>
       </c>
@@ -2927,7 +2963,7 @@
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
     </row>
-    <row r="32" spans="2:16" ht="36" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
         <v>269</v>
       </c>
@@ -2964,7 +3000,7 @@
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
         <v>269</v>
       </c>
@@ -3001,7 +3037,7 @@
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
     </row>
-    <row r="34" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
         <v>269</v>
       </c>
@@ -3040,7 +3076,7 @@
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
     </row>
-    <row r="35" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
         <v>269</v>
       </c>
@@ -3077,7 +3113,7 @@
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
     </row>
-    <row r="36" spans="2:16" ht="48" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" ht="48" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>269</v>
       </c>
@@ -3118,7 +3154,7 @@
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
     </row>
-    <row r="37" spans="2:16" ht="36" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
         <v>269</v>
       </c>
@@ -3159,7 +3195,7 @@
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
-    <row r="38" spans="2:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
         <v>269</v>
       </c>
@@ -3198,7 +3234,7 @@
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
     </row>
-    <row r="39" spans="2:16" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
         <v>269</v>
       </c>
@@ -3233,7 +3269,7 @@
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
     </row>
-    <row r="40" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
         <v>269</v>
       </c>
@@ -3268,7 +3304,7 @@
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
     </row>
-    <row r="41" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
         <v>269</v>
       </c>
@@ -3307,7 +3343,7 @@
       <c r="O41" s="5"/>
       <c r="P41" s="5"/>
     </row>
-    <row r="42" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
         <v>269</v>
       </c>
@@ -3344,7 +3380,7 @@
       <c r="O42" s="5"/>
       <c r="P42" s="5"/>
     </row>
-    <row r="43" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
         <v>269</v>
       </c>
@@ -3381,7 +3417,7 @@
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
     </row>
-    <row r="44" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
         <v>269</v>
       </c>
@@ -3416,7 +3452,7 @@
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
     </row>
-    <row r="45" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
         <v>269</v>
       </c>
@@ -3451,7 +3487,7 @@
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
     </row>
-    <row r="46" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
         <v>269</v>
       </c>
@@ -3481,12 +3517,14 @@
       <c r="L46" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="M46" s="14"/>
+      <c r="M46" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
     </row>
-    <row r="47" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
         <v>269</v>
       </c>
@@ -3516,12 +3554,14 @@
       <c r="L47" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="M47" s="14"/>
+      <c r="M47" s="14" t="s">
+        <v>321</v>
+      </c>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
     </row>
-    <row r="48" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B48" s="6" t="s">
         <v>269</v>
       </c>
@@ -3553,12 +3593,14 @@
       <c r="L48" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="M48" s="14"/>
+      <c r="M48" s="14" t="s">
+        <v>322</v>
+      </c>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
     </row>
-    <row r="49" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B49" s="6" t="s">
         <v>269</v>
       </c>
@@ -3593,7 +3635,7 @@
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
     </row>
-    <row r="50" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B50" s="6" t="s">
         <v>269</v>
       </c>
@@ -3623,12 +3665,14 @@
       <c r="L50" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="M50" s="14"/>
+      <c r="M50" s="14" t="s">
+        <v>323</v>
+      </c>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
     </row>
-    <row r="51" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B51" s="6" t="s">
         <v>269</v>
       </c>
@@ -3667,7 +3711,7 @@
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B52" s="6" t="s">
         <v>269</v>
       </c>
@@ -3704,7 +3748,7 @@
       <c r="O52" s="5"/>
       <c r="P52" s="5"/>
     </row>
-    <row r="53" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B53" s="6" t="s">
         <v>269</v>
       </c>
@@ -3743,7 +3787,7 @@
       <c r="O53" s="5"/>
       <c r="P53" s="5"/>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B54" s="6" t="s">
         <v>269</v>
       </c>
@@ -3780,7 +3824,7 @@
       <c r="O54" s="5"/>
       <c r="P54" s="5"/>
     </row>
-    <row r="55" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B55" s="6" t="s">
         <v>269</v>
       </c>
@@ -3812,12 +3856,14 @@
       <c r="L55" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="M55" s="14"/>
+      <c r="M55" s="14" t="s">
+        <v>324</v>
+      </c>
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
     </row>
-    <row r="56" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B56" s="6" t="s">
         <v>269</v>
       </c>
@@ -3852,7 +3898,7 @@
       <c r="O56" s="5"/>
       <c r="P56" s="5"/>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B57" s="6" t="s">
         <v>269</v>
       </c>
@@ -3887,7 +3933,7 @@
       <c r="O57" s="5"/>
       <c r="P57" s="5"/>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B58" s="6" t="s">
         <v>269</v>
       </c>
@@ -3922,7 +3968,7 @@
       <c r="O58" s="5"/>
       <c r="P58" s="5"/>
     </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B59" s="6" t="s">
         <v>269</v>
       </c>
@@ -3957,7 +4003,7 @@
       <c r="O59" s="5"/>
       <c r="P59" s="5"/>
     </row>
-    <row r="60" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B60" s="9" t="s">
         <v>271</v>
       </c>
@@ -3988,7 +4034,7 @@
       <c r="O60" s="5"/>
       <c r="P60" s="5"/>
     </row>
-    <row r="61" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" s="9" t="s">
         <v>271</v>
       </c>
@@ -4019,7 +4065,7 @@
       <c r="O61" s="5"/>
       <c r="P61" s="5"/>
     </row>
-    <row r="62" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B62" s="9" t="s">
         <v>271</v>
       </c>
@@ -4050,7 +4096,7 @@
       <c r="O62" s="5"/>
       <c r="P62" s="5"/>
     </row>
-    <row r="63" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B63" s="9" t="s">
         <v>271</v>
       </c>
@@ -4081,7 +4127,7 @@
       <c r="O63" s="5"/>
       <c r="P63" s="5"/>
     </row>
-    <row r="64" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B64" s="9" t="s">
         <v>271</v>
       </c>
@@ -4112,7 +4158,7 @@
       <c r="O64" s="5"/>
       <c r="P64" s="5"/>
     </row>
-    <row r="65" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B65" s="9" t="s">
         <v>271</v>
       </c>
@@ -4141,7 +4187,7 @@
       <c r="O65" s="5"/>
       <c r="P65" s="5"/>
     </row>
-    <row r="66" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B66" s="9" t="s">
         <v>271</v>
       </c>
@@ -4172,7 +4218,7 @@
       <c r="O66" s="5"/>
       <c r="P66" s="5"/>
     </row>
-    <row r="67" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B67" s="9" t="s">
         <v>271</v>
       </c>
@@ -4203,7 +4249,7 @@
       <c r="O67" s="5"/>
       <c r="P67" s="5"/>
     </row>
-    <row r="68" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B68" s="6" t="s">
         <v>269</v>
       </c>
@@ -4238,7 +4284,7 @@
       <c r="O68" s="5"/>
       <c r="P68" s="5"/>
     </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B69" s="6" t="s">
         <v>269</v>
       </c>
@@ -4273,7 +4319,7 @@
       <c r="O69" s="5"/>
       <c r="P69" s="5"/>
     </row>
-    <row r="70" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B70" s="9" t="s">
         <v>271</v>
       </c>
@@ -4306,7 +4352,7 @@
       <c r="O70" s="5"/>
       <c r="P70" s="5"/>
     </row>
-    <row r="71" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B71" s="9" t="s">
         <v>271</v>
       </c>
@@ -4339,7 +4385,7 @@
       <c r="O71" s="5"/>
       <c r="P71" s="5"/>
     </row>
-    <row r="72" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B72" s="9" t="s">
         <v>271</v>
       </c>
@@ -4370,7 +4416,7 @@
       <c r="O72" s="5"/>
       <c r="P72" s="5"/>
     </row>
-    <row r="73" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B73" s="9" t="s">
         <v>271</v>
       </c>
@@ -4401,7 +4447,7 @@
       <c r="O73" s="5"/>
       <c r="P73" s="5"/>
     </row>
-    <row r="74" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B74" s="9" t="s">
         <v>271</v>
       </c>
@@ -4434,7 +4480,7 @@
       <c r="O74" s="5"/>
       <c r="P74" s="5"/>
     </row>
-    <row r="75" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B75" s="9" t="s">
         <v>271</v>
       </c>
@@ -4467,7 +4513,7 @@
       <c r="O75" s="5"/>
       <c r="P75" s="5"/>
     </row>
-    <row r="76" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B76" s="9" t="s">
         <v>271</v>
       </c>
@@ -4500,7 +4546,7 @@
       <c r="O76" s="5"/>
       <c r="P76" s="5"/>
     </row>
-    <row r="77" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B77" s="9" t="s">
         <v>271</v>
       </c>
@@ -4531,7 +4577,7 @@
       <c r="O77" s="5"/>
       <c r="P77" s="5"/>
     </row>
-    <row r="78" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B78" s="9" t="s">
         <v>271</v>
       </c>
@@ -4562,7 +4608,7 @@
       <c r="O78" s="5"/>
       <c r="P78" s="5"/>
     </row>
-    <row r="79" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B79" s="9" t="s">
         <v>271</v>
       </c>
@@ -4595,7 +4641,7 @@
       <c r="O79" s="5"/>
       <c r="P79" s="5"/>
     </row>
-    <row r="80" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B80" s="9" t="s">
         <v>271</v>
       </c>
@@ -4628,7 +4674,7 @@
       <c r="O80" s="5"/>
       <c r="P80" s="5"/>
     </row>
-    <row r="81" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B81" s="9" t="s">
         <v>271</v>
       </c>
@@ -4661,7 +4707,7 @@
       <c r="O81" s="5"/>
       <c r="P81" s="5"/>
     </row>
-    <row r="82" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B82" s="9" t="s">
         <v>271</v>
       </c>
@@ -4692,7 +4738,7 @@
       <c r="O82" s="5"/>
       <c r="P82" s="5"/>
     </row>
-    <row r="83" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B83" s="9" t="s">
         <v>271</v>
       </c>
@@ -4723,7 +4769,7 @@
       <c r="O83" s="5"/>
       <c r="P83" s="5"/>
     </row>
-    <row r="84" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B84" s="9" t="s">
         <v>271</v>
       </c>
@@ -4756,7 +4802,7 @@
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
     </row>
-    <row r="85" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B85" s="9" t="s">
         <v>271</v>
       </c>
@@ -4789,7 +4835,7 @@
       <c r="O85" s="5"/>
       <c r="P85" s="5"/>
     </row>
-    <row r="86" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B86" s="9" t="s">
         <v>271</v>
       </c>
@@ -4822,7 +4868,7 @@
       <c r="O86" s="5"/>
       <c r="P86" s="5"/>
     </row>
-    <row r="87" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B87" s="9" t="s">
         <v>271</v>
       </c>
@@ -4853,7 +4899,7 @@
       <c r="O87" s="5"/>
       <c r="P87" s="5"/>
     </row>
-    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B88" s="6" t="s">
         <v>269</v>
       </c>
@@ -4888,7 +4934,7 @@
       <c r="O88" s="5"/>
       <c r="P88" s="5"/>
     </row>
-    <row r="89" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B89" s="6" t="s">
         <v>269</v>
       </c>
@@ -4923,7 +4969,7 @@
       <c r="O89" s="5"/>
       <c r="P89" s="5"/>
     </row>
-    <row r="90" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B90" s="6" t="s">
         <v>269</v>
       </c>
@@ -4958,7 +5004,7 @@
       <c r="O90" s="5"/>
       <c r="P90" s="5"/>
     </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B91" s="6" t="s">
         <v>269</v>
       </c>
@@ -4997,7 +5043,7 @@
       <c r="O91" s="5"/>
       <c r="P91" s="5"/>
     </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B92" s="6" t="s">
         <v>269</v>
       </c>
@@ -5036,7 +5082,7 @@
       <c r="O92" s="5"/>
       <c r="P92" s="5"/>
     </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B93" s="6" t="s">
         <v>269</v>
       </c>
@@ -5075,7 +5121,7 @@
       <c r="O93" s="5"/>
       <c r="P93" s="5"/>
     </row>
-    <row r="94" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="B94" s="9" t="s">
         <v>271</v>
       </c>
@@ -5106,7 +5152,7 @@
       <c r="O94" s="5"/>
       <c r="P94" s="5"/>
     </row>
-    <row r="95" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B95" s="9" t="s">
         <v>271</v>
       </c>
@@ -5137,7 +5183,7 @@
       <c r="O95" s="5"/>
       <c r="P95" s="5"/>
     </row>
-    <row r="96" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="B96" s="9" t="s">
         <v>271</v>
       </c>
@@ -5168,7 +5214,7 @@
       <c r="O96" s="5"/>
       <c r="P96" s="5"/>
     </row>
-    <row r="97" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="B97" s="9" t="s">
         <v>271</v>
       </c>
@@ -5199,7 +5245,7 @@
       <c r="O97" s="5"/>
       <c r="P97" s="5"/>
     </row>
-    <row r="98" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="B98" s="9" t="s">
         <v>271</v>
       </c>
@@ -5230,7 +5276,7 @@
       <c r="O98" s="5"/>
       <c r="P98" s="5"/>
     </row>
-    <row r="99" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="B99" s="9" t="s">
         <v>271</v>
       </c>
@@ -5261,7 +5307,7 @@
       <c r="O99" s="5"/>
       <c r="P99" s="5"/>
     </row>
-    <row r="100" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:20" x14ac:dyDescent="0.2">
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
       <c r="J100" s="5"/>

</xml_diff>

<commit_message>
Final excel files for GREEN (iApply Light) version
</commit_message>
<xml_diff>
--- a/iApply_CCBS_Interfaces.xlsx
+++ b/iApply_CCBS_Interfaces.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20401"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF0986A-2E85-4A69-A86F-C9FBA1CF6F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79945079-9C8D-463B-B6B4-47BEAC4F1060}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11025" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CCBS_API_CALLS" sheetId="5" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="338">
   <si>
     <t>INSERT</t>
   </si>
@@ -1047,13 +1047,16 @@
   </si>
   <si>
     <t>Mortgages_Update.xlsx</t>
+  </si>
+  <si>
+    <t>Exposures_DownloadDepts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1124,6 +1127,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1138,7 +1148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1160,12 +1170,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1246,23 +1250,23 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1553,11 +1557,6 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:P93">
-    <sortCondition ref="F3:F99"/>
-    <sortCondition ref="G3:G99"/>
-    <sortCondition ref="C3:C99"/>
-  </sortState>
   <tableColumns count="15">
     <tableColumn id="5" xr3:uid="{439C2326-B5B7-468F-998C-E1E2D33178F2}" name="Color" dataDxfId="14"/>
     <tableColumn id="7" xr3:uid="{E6F3ECB4-BA57-46DA-9083-F5256AC0F6BA}" name="Group" dataDxfId="13"/>
@@ -1580,9 +1579,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1620,9 +1619,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1655,9 +1654,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1690,9 +1706,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1873,35 +1906,35 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.5546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.33203125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="8.88671875" style="2"/>
-    <col min="18" max="18" width="14.44140625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" style="2"/>
-    <col min="20" max="20" width="14.44140625" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="1.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.5703125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" style="2"/>
+    <col min="18" max="18" width="14.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" style="2"/>
+    <col min="20" max="20" width="14.42578125" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="8.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
       <c r="C1" s="17">
         <v>3</v>
@@ -1920,7 +1953,7 @@
       <c r="M1" s="3"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="2:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>272</v>
       </c>
@@ -1967,128 +2000,124 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="48" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>309</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="E3" s="15"/>
       <c r="F3" s="4">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>268</v>
+      </c>
       <c r="K3" s="4">
         <v>1</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>207</v>
+        <v>100</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>309</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="E4" s="15"/>
       <c r="F4" s="4">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>266</v>
+      </c>
       <c r="K4" s="4">
         <v>1</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="2:16" ht="36" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>309</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="E5" s="15"/>
       <c r="F5" s="4">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="K5" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>278</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>270</v>
       </c>
@@ -2123,7 +2152,7 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="2:16" ht="48" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>269</v>
       </c>
@@ -2133,83 +2162,77 @@
       <c r="D7" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>308</v>
-      </c>
+      <c r="E7" s="15"/>
       <c r="F7" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="K7" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="2:16" ht="48" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" ht="48" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>308</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="E8" s="15"/>
       <c r="F8" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>108</v>
+        <v>193</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>21</v>
+        <v>192</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="K8" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>295</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="2:16" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>269</v>
       </c>
@@ -2219,149 +2242,149 @@
       <c r="D9" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>308</v>
-      </c>
+      <c r="E9" s="15"/>
       <c r="F9" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="K9" s="4">
-        <v>1</v>
-      </c>
-      <c r="L9" s="15"/>
+        <v>3</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>0</v>
+      </c>
       <c r="M9" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="N9" s="5"/>
+        <v>311</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>293</v>
+      </c>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>309</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="E10" s="15"/>
       <c r="F10" s="4">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="4">
         <v>1</v>
       </c>
-      <c r="L10" s="16"/>
-      <c r="M10" s="5" t="s">
-        <v>223</v>
+      <c r="L10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>331</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>319</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="E11" s="15"/>
       <c r="F11" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="4">
         <v>1</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>319</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E12" s="15"/>
       <c r="F12" s="4">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="4">
         <v>1</v>
       </c>
-      <c r="L12" s="16"/>
-      <c r="M12" s="5" t="s">
-        <v>227</v>
+      <c r="L12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>325</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>270</v>
       </c>
@@ -2394,48 +2417,44 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>319</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E14" s="15"/>
       <c r="F14" s="4">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>134</v>
+        <v>186</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>265</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="J14" s="5"/>
       <c r="K14" s="4">
         <v>1</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>226</v>
+        <v>2</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>326</v>
       </c>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
         <v>270</v>
       </c>
@@ -2468,46 +2487,44 @@
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>205</v>
+        <v>100</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>319</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="E16" s="15"/>
       <c r="F16" s="4">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>260</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="J16" s="5"/>
       <c r="K16" s="4">
         <v>1</v>
       </c>
-      <c r="L16" s="16"/>
+      <c r="L16" s="15" t="s">
+        <v>2</v>
+      </c>
       <c r="M16" s="5" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="2:16" ht="36" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
         <v>269</v>
       </c>
@@ -2522,33 +2539,29 @@
         <v>4</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>254</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J17" s="5"/>
       <c r="K17" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L17" s="15" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="N17" s="5" t="s">
-        <v>279</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" s="9" t="s">
         <v>271</v>
       </c>
@@ -2579,7 +2592,7 @@
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
-    <row r="19" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B19" s="9" t="s">
         <v>271</v>
       </c>
@@ -2610,7 +2623,7 @@
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
     </row>
-    <row r="20" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" s="9" t="s">
         <v>271</v>
       </c>
@@ -2641,7 +2654,7 @@
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B21" s="9" t="s">
         <v>271</v>
       </c>
@@ -2672,7 +2685,7 @@
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
     </row>
-    <row r="22" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" s="9" t="s">
         <v>271</v>
       </c>
@@ -2703,7 +2716,7 @@
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" s="9" t="s">
         <v>271</v>
       </c>
@@ -2734,7 +2747,7 @@
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B24" s="9" t="s">
         <v>271</v>
       </c>
@@ -2765,7 +2778,7 @@
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
         <v>271</v>
       </c>
@@ -2796,7 +2809,7 @@
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" s="9" t="s">
         <v>271</v>
       </c>
@@ -2827,7 +2840,7 @@
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B27" s="9" t="s">
         <v>271</v>
       </c>
@@ -2858,7 +2871,7 @@
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
     </row>
-    <row r="28" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" s="9" t="s">
         <v>271</v>
       </c>
@@ -2889,7 +2902,7 @@
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
     </row>
-    <row r="29" spans="2:16" ht="36" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
         <v>269</v>
       </c>
@@ -2904,33 +2917,29 @@
         <v>4</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>254</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="J29" s="5"/>
       <c r="K29" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L29" s="15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="N29" s="5" t="s">
-        <v>293</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
     </row>
-    <row r="30" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
         <v>269</v>
       </c>
@@ -2945,13 +2954,13 @@
         <v>4</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="4">
@@ -2961,282 +2970,284 @@
         <v>2</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
     </row>
-    <row r="31" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>282</v>
+        <v>303</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="4">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>112</v>
+        <v>189</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="4">
         <v>1</v>
       </c>
       <c r="L31" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>220</v>
+        <v>2</v>
+      </c>
+      <c r="M31" s="14" t="s">
+        <v>333</v>
       </c>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
     </row>
-    <row r="32" spans="2:16" ht="36" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" ht="60" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E32" s="15"/>
+        <v>283</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>309</v>
+      </c>
       <c r="F32" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="4">
         <v>1</v>
       </c>
       <c r="L32" s="15" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>282</v>
+        <v>315</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="4">
         <v>1</v>
       </c>
       <c r="L33" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>219</v>
+        <v>3</v>
+      </c>
+      <c r="M33" s="14" t="s">
+        <v>337</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
     </row>
-    <row r="34" spans="2:16" s="26" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" s="27" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C34" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="D34" s="23" t="s">
-        <v>282</v>
-      </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="25">
-        <v>4</v>
-      </c>
-      <c r="G34" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="H34" s="25" t="s">
+      <c r="C34" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="I34" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J34" s="22" t="s">
-        <v>258</v>
-      </c>
-      <c r="K34" s="25">
-        <v>1</v>
-      </c>
-      <c r="L34" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M34" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-    </row>
-    <row r="35" spans="2:16" ht="24" x14ac:dyDescent="0.25">
-      <c r="B35" s="27" t="s">
+      <c r="I34" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J34" s="5"/>
+      <c r="K34" s="4">
+        <v>1</v>
+      </c>
+      <c r="L34" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="2:16" ht="36" x14ac:dyDescent="0.2">
+      <c r="B35" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E35" s="15"/>
+        <v>283</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>309</v>
+      </c>
       <c r="F35" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J35" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>259</v>
+      </c>
       <c r="K35" s="4">
         <v>2</v>
       </c>
       <c r="L35" s="15" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="N35" s="5"/>
+        <v>314</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>278</v>
+      </c>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
     </row>
-    <row r="36" spans="2:16" ht="48" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E36" s="15"/>
+        <v>284</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>319</v>
+      </c>
       <c r="F36" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>255</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="J36" s="5"/>
       <c r="K36" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L36" s="15" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="N36" s="5" t="s">
-        <v>296</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
     </row>
-    <row r="37" spans="2:16" ht="36" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E37" s="15"/>
+        <v>284</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>319</v>
+      </c>
       <c r="F37" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>255</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="J37" s="5"/>
       <c r="K37" s="4">
-        <v>3</v>
-      </c>
-      <c r="L37" s="15" t="s">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L37" s="16"/>
       <c r="M37" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="N37" s="5" t="s">
-        <v>297</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
-    <row r="38" spans="2:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
         <v>269</v>
       </c>
@@ -3244,38 +3255,40 @@
         <v>205</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="E38" s="15"/>
+        <v>284</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>319</v>
+      </c>
       <c r="F38" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>193</v>
+        <v>134</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>192</v>
+        <v>52</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="K38" s="4">
         <v>1</v>
       </c>
       <c r="L38" s="15" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
     </row>
-    <row r="39" spans="2:16" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
         <v>269</v>
       </c>
@@ -3283,219 +3296,235 @@
         <v>205</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="E39" s="15"/>
+        <v>284</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>319</v>
+      </c>
       <c r="F39" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J39" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>260</v>
+      </c>
       <c r="K39" s="4">
         <v>1</v>
       </c>
-      <c r="L39" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="M39" s="28"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
     </row>
-    <row r="40" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E40" s="15"/>
       <c r="F40" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>123</v>
+        <v>199</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="4">
         <v>1</v>
       </c>
-      <c r="L40" s="16"/>
-      <c r="M40" s="5" t="s">
-        <v>237</v>
+      <c r="L40" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M40" s="14" t="s">
+        <v>320</v>
       </c>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
     </row>
-    <row r="41" spans="2:16" ht="24" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="s">
+    <row r="41" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+      <c r="B41" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="4">
-        <v>6</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H41" s="4" t="s">
+      <c r="C41" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="E41" s="25"/>
+      <c r="F41" s="26">
+        <v>4</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="H41" s="26" t="s">
         <v>287</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="K41" s="4">
-        <v>1</v>
-      </c>
-      <c r="L41" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-    </row>
-    <row r="42" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+      <c r="I41" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J41" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="K41" s="26">
+        <v>1</v>
+      </c>
+      <c r="L41" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="M41" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="N41" s="23"/>
+      <c r="O41" s="23"/>
+      <c r="P41" s="23"/>
+    </row>
+    <row r="42" spans="2:16" ht="48" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E42" s="15"/>
+        <v>282</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>308</v>
+      </c>
       <c r="F42" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J42" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>256</v>
+      </c>
       <c r="K42" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L42" s="15" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="N42" s="5"/>
+        <v>305</v>
+      </c>
+      <c r="N42" s="5" t="s">
+        <v>294</v>
+      </c>
       <c r="O42" s="5"/>
       <c r="P42" s="5"/>
     </row>
-    <row r="43" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" ht="48" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>101</v>
+        <v>206</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E43" s="15"/>
+        <v>282</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>308</v>
+      </c>
       <c r="F43" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>191</v>
+        <v>108</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="J43" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>257</v>
+      </c>
       <c r="K43" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L43" s="15" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="N43" s="5"/>
+        <v>306</v>
+      </c>
+      <c r="N43" s="5" t="s">
+        <v>295</v>
+      </c>
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
     </row>
-    <row r="44" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E44" s="15"/>
       <c r="F44" s="4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>182</v>
+        <v>123</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="4">
         <v>1</v>
       </c>
-      <c r="L44" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="M44" s="14" t="s">
-        <v>325</v>
+      <c r="L44" s="16"/>
+      <c r="M44" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
     </row>
-    <row r="45" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
         <v>269</v>
       </c>
@@ -3510,52 +3539,54 @@
         <v>10</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="4">
         <v>1</v>
       </c>
       <c r="L45" s="15" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M45" s="14" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
     </row>
-    <row r="46" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="4">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>199</v>
+        <v>130</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="J46" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>261</v>
+      </c>
       <c r="K46" s="4">
         <v>1</v>
       </c>
@@ -3563,34 +3594,34 @@
         <v>0</v>
       </c>
       <c r="M46" s="14" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
     </row>
-    <row r="47" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>212</v>
+        <v>101</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>300</v>
+        <v>101</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>90</v>
+        <v>304</v>
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="4">
@@ -3599,14 +3630,14 @@
       <c r="L47" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="M47" s="14" t="s">
-        <v>321</v>
+      <c r="M47" s="5" t="s">
+        <v>225</v>
       </c>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
     </row>
-    <row r="48" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B48" s="6" t="s">
         <v>269</v>
       </c>
@@ -3645,44 +3676,44 @@
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
     </row>
-    <row r="49" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B49" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="E49" s="15"/>
       <c r="F49" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="J49" s="5"/>
       <c r="K49" s="4">
         <v>1</v>
       </c>
       <c r="L49" s="15" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M49" s="14" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
     </row>
-    <row r="50" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B50" s="6" t="s">
         <v>269</v>
       </c>
@@ -3697,29 +3728,29 @@
         <v>10</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J50" s="5"/>
       <c r="K50" s="4">
         <v>1</v>
       </c>
       <c r="L50" s="15" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M50" s="14" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
     </row>
-    <row r="51" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B51" s="6" t="s">
         <v>269</v>
       </c>
@@ -3734,92 +3765,92 @@
         <v>12</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="K51" s="4">
         <v>1</v>
       </c>
       <c r="L51" s="15" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B52" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>100</v>
+        <v>208</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E52" s="15"/>
       <c r="F52" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>39</v>
+        <v>291</v>
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="4">
         <v>1</v>
       </c>
       <c r="L52" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="M52" s="5" t="s">
-        <v>240</v>
+        <v>3</v>
+      </c>
+      <c r="M52" s="14" t="s">
+        <v>328</v>
       </c>
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
       <c r="P52" s="5"/>
     </row>
-    <row r="53" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B53" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>100</v>
+        <v>205</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E53" s="15"/>
       <c r="F53" s="4">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>129</v>
+        <v>214</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>40</v>
+        <v>194</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="K53" s="4">
         <v>1</v>
@@ -3828,74 +3859,74 @@
         <v>3</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
       <c r="P53" s="5"/>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B54" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="E54" s="15"/>
       <c r="F54" s="4">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>127</v>
+        <v>190</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="J54" s="5"/>
       <c r="K54" s="4">
         <v>1</v>
       </c>
       <c r="L54" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M54" s="5" t="s">
-        <v>239</v>
+        <v>3</v>
+      </c>
+      <c r="M54" s="14" t="s">
+        <v>335</v>
       </c>
       <c r="N54" s="5"/>
       <c r="O54" s="5"/>
       <c r="P54" s="5"/>
     </row>
-    <row r="55" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B55" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>302</v>
+        <v>315</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="4">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="K55" s="4">
         <v>1</v>
@@ -3903,162 +3934,164 @@
       <c r="L55" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="M55" s="14" t="s">
-        <v>324</v>
+      <c r="M55" s="5" t="s">
+        <v>230</v>
       </c>
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
     </row>
-    <row r="56" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B56" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="E56" s="15"/>
       <c r="F56" s="4">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>291</v>
+        <v>53</v>
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="4">
         <v>1</v>
       </c>
       <c r="L56" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="M56" s="14" t="s">
-        <v>328</v>
+        <v>12</v>
+      </c>
+      <c r="M56" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="N56" s="5"/>
       <c r="O56" s="5"/>
       <c r="P56" s="5"/>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B57" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="E57" s="15"/>
+        <v>282</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>308</v>
+      </c>
       <c r="F57" s="4">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J57" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>253</v>
+      </c>
       <c r="K57" s="4">
         <v>1</v>
       </c>
-      <c r="L57" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M57" s="14" t="s">
-        <v>329</v>
+      <c r="L57" s="15"/>
+      <c r="M57" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="N57" s="5"/>
       <c r="O57" s="5"/>
       <c r="P57" s="5"/>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B58" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="E58" s="15"/>
+        <v>283</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>309</v>
+      </c>
       <c r="F58" s="4">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J58" s="5"/>
       <c r="K58" s="4">
         <v>1</v>
       </c>
-      <c r="L58" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="M58" s="14" t="s">
-        <v>330</v>
+      <c r="L58" s="16"/>
+      <c r="M58" s="5" t="s">
+        <v>223</v>
       </c>
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
       <c r="P58" s="5"/>
     </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B59" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E59" s="15"/>
       <c r="F59" s="4">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>113</v>
+        <v>185</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="J59" s="5"/>
       <c r="K59" s="4">
         <v>1</v>
       </c>
       <c r="L59" s="15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M59" s="14" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="N59" s="5"/>
       <c r="O59" s="5"/>
       <c r="P59" s="5"/>
     </row>
-    <row r="60" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B60" s="9" t="s">
         <v>271</v>
       </c>
@@ -4089,7 +4122,7 @@
       <c r="O60" s="5"/>
       <c r="P60" s="5"/>
     </row>
-    <row r="61" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" s="9" t="s">
         <v>271</v>
       </c>
@@ -4120,7 +4153,7 @@
       <c r="O61" s="5"/>
       <c r="P61" s="5"/>
     </row>
-    <row r="62" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B62" s="9" t="s">
         <v>271</v>
       </c>
@@ -4151,7 +4184,7 @@
       <c r="O62" s="5"/>
       <c r="P62" s="5"/>
     </row>
-    <row r="63" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B63" s="9" t="s">
         <v>271</v>
       </c>
@@ -4182,7 +4215,7 @@
       <c r="O63" s="5"/>
       <c r="P63" s="5"/>
     </row>
-    <row r="64" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B64" s="9" t="s">
         <v>271</v>
       </c>
@@ -4213,7 +4246,7 @@
       <c r="O64" s="5"/>
       <c r="P64" s="5"/>
     </row>
-    <row r="65" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B65" s="9" t="s">
         <v>271</v>
       </c>
@@ -4242,7 +4275,7 @@
       <c r="O65" s="5"/>
       <c r="P65" s="5"/>
     </row>
-    <row r="66" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B66" s="9" t="s">
         <v>271</v>
       </c>
@@ -4273,7 +4306,7 @@
       <c r="O66" s="5"/>
       <c r="P66" s="5"/>
     </row>
-    <row r="67" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B67" s="9" t="s">
         <v>271</v>
       </c>
@@ -4304,28 +4337,28 @@
       <c r="O67" s="5"/>
       <c r="P67" s="5"/>
     </row>
-    <row r="68" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B68" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>204</v>
+        <v>100</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="E68" s="15"/>
       <c r="F68" s="4">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="H68" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="J68" s="5"/>
       <c r="K68" s="4">
@@ -4334,51 +4367,51 @@
       <c r="L68" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="M68" s="14" t="s">
-        <v>332</v>
+      <c r="M68" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
       <c r="P68" s="5"/>
     </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B69" s="6" t="s">
+    <row r="69" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+      <c r="B69" s="28" t="s">
         <v>269</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D69" s="20" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="E69" s="15"/>
       <c r="F69" s="4">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>189</v>
+        <v>110</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="J69" s="5"/>
       <c r="K69" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L69" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="M69" s="14" t="s">
-        <v>333</v>
+        <v>0</v>
+      </c>
+      <c r="M69" s="5" t="s">
+        <v>216</v>
       </c>
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
       <c r="P69" s="5"/>
     </row>
-    <row r="70" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B70" s="9" t="s">
         <v>271</v>
       </c>
@@ -4411,7 +4444,7 @@
       <c r="O70" s="5"/>
       <c r="P70" s="5"/>
     </row>
-    <row r="71" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B71" s="9" t="s">
         <v>271</v>
       </c>
@@ -4444,7 +4477,7 @@
       <c r="O71" s="5"/>
       <c r="P71" s="5"/>
     </row>
-    <row r="72" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B72" s="9" t="s">
         <v>271</v>
       </c>
@@ -4475,7 +4508,7 @@
       <c r="O72" s="5"/>
       <c r="P72" s="5"/>
     </row>
-    <row r="73" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B73" s="9" t="s">
         <v>271</v>
       </c>
@@ -4506,7 +4539,7 @@
       <c r="O73" s="5"/>
       <c r="P73" s="5"/>
     </row>
-    <row r="74" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B74" s="9" t="s">
         <v>271</v>
       </c>
@@ -4539,7 +4572,7 @@
       <c r="O74" s="5"/>
       <c r="P74" s="5"/>
     </row>
-    <row r="75" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B75" s="9" t="s">
         <v>271</v>
       </c>
@@ -4572,7 +4605,7 @@
       <c r="O75" s="5"/>
       <c r="P75" s="5"/>
     </row>
-    <row r="76" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B76" s="9" t="s">
         <v>271</v>
       </c>
@@ -4605,7 +4638,7 @@
       <c r="O76" s="5"/>
       <c r="P76" s="5"/>
     </row>
-    <row r="77" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B77" s="9" t="s">
         <v>271</v>
       </c>
@@ -4636,7 +4669,7 @@
       <c r="O77" s="5"/>
       <c r="P77" s="5"/>
     </row>
-    <row r="78" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B78" s="9" t="s">
         <v>271</v>
       </c>
@@ -4667,7 +4700,7 @@
       <c r="O78" s="5"/>
       <c r="P78" s="5"/>
     </row>
-    <row r="79" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B79" s="9" t="s">
         <v>271</v>
       </c>
@@ -4700,7 +4733,7 @@
       <c r="O79" s="5"/>
       <c r="P79" s="5"/>
     </row>
-    <row r="80" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B80" s="9" t="s">
         <v>271</v>
       </c>
@@ -4733,7 +4766,7 @@
       <c r="O80" s="5"/>
       <c r="P80" s="5"/>
     </row>
-    <row r="81" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B81" s="9" t="s">
         <v>271</v>
       </c>
@@ -4766,7 +4799,7 @@
       <c r="O81" s="5"/>
       <c r="P81" s="5"/>
     </row>
-    <row r="82" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B82" s="9" t="s">
         <v>271</v>
       </c>
@@ -4797,7 +4830,7 @@
       <c r="O82" s="5"/>
       <c r="P82" s="5"/>
     </row>
-    <row r="83" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B83" s="9" t="s">
         <v>271</v>
       </c>
@@ -4828,7 +4861,7 @@
       <c r="O83" s="5"/>
       <c r="P83" s="5"/>
     </row>
-    <row r="84" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B84" s="9" t="s">
         <v>271</v>
       </c>
@@ -4861,7 +4894,7 @@
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
     </row>
-    <row r="85" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B85" s="9" t="s">
         <v>271</v>
       </c>
@@ -4894,7 +4927,7 @@
       <c r="O85" s="5"/>
       <c r="P85" s="5"/>
     </row>
-    <row r="86" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B86" s="9" t="s">
         <v>271</v>
       </c>
@@ -4927,7 +4960,7 @@
       <c r="O86" s="5"/>
       <c r="P86" s="5"/>
     </row>
-    <row r="87" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B87" s="9" t="s">
         <v>271</v>
       </c>
@@ -4958,235 +4991,237 @@
       <c r="O87" s="5"/>
       <c r="P87" s="5"/>
     </row>
-    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B88" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D88" s="20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E88" s="15"/>
       <c r="F88" s="4">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I88" s="5" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="J88" s="5"/>
       <c r="K88" s="4">
         <v>1</v>
       </c>
       <c r="L88" s="15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M88" s="14" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="N88" s="5"/>
       <c r="O88" s="5"/>
       <c r="P88" s="5"/>
     </row>
-    <row r="89" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B89" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D89" s="20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E89" s="15"/>
       <c r="F89" s="4">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>190</v>
+        <v>133</v>
       </c>
       <c r="H89" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="J89" s="5"/>
       <c r="K89" s="4">
         <v>1</v>
       </c>
       <c r="L89" s="15" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="M89" s="14" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="N89" s="5"/>
       <c r="O89" s="5"/>
       <c r="P89" s="5"/>
     </row>
-    <row r="90" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:16" ht="48" x14ac:dyDescent="0.2">
       <c r="B90" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D90" s="20" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="E90" s="15"/>
       <c r="F90" s="4">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>188</v>
+        <v>104</v>
       </c>
       <c r="H90" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="J90" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="J90" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="K90" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L90" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="M90" s="14" t="s">
-        <v>336</v>
-      </c>
-      <c r="N90" s="5"/>
+      <c r="M90" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="N90" s="5" t="s">
+        <v>296</v>
+      </c>
       <c r="O90" s="5"/>
       <c r="P90" s="5"/>
     </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:16" ht="36" x14ac:dyDescent="0.2">
       <c r="B91" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="E91" s="15"/>
       <c r="F91" s="4">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="H91" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="K91" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L91" s="15" t="s">
         <v>1</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="N91" s="5"/>
+        <v>313</v>
+      </c>
+      <c r="N91" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="O91" s="5"/>
       <c r="P91" s="5"/>
     </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B92" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D92" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E92" s="15"/>
       <c r="F92" s="4">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="H92" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I92" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J92" s="5" t="s">
-        <v>268</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="J92" s="5"/>
       <c r="K92" s="4">
         <v>1</v>
       </c>
       <c r="L92" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="M92" s="5" t="s">
-        <v>234</v>
+        <v>1</v>
+      </c>
+      <c r="M92" s="14" t="s">
+        <v>332</v>
       </c>
       <c r="N92" s="5"/>
       <c r="O92" s="5"/>
       <c r="P92" s="5"/>
     </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:16" ht="24" x14ac:dyDescent="0.2">
       <c r="B93" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D93" s="20" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="E93" s="15"/>
       <c r="F93" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="H93" s="4" t="s">
         <v>287</v>
       </c>
       <c r="I93" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="J93" s="5" t="s">
-        <v>268</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="J93" s="5"/>
       <c r="K93" s="4">
         <v>1</v>
       </c>
       <c r="L93" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="M93" s="5" t="s">
-        <v>235</v>
+        <v>1</v>
+      </c>
+      <c r="M93" s="14" t="s">
+        <v>336</v>
       </c>
       <c r="N93" s="5"/>
       <c r="O93" s="5"/>
       <c r="P93" s="5"/>
     </row>
-    <row r="94" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="B94" s="9" t="s">
         <v>271</v>
       </c>
@@ -5217,7 +5252,7 @@
       <c r="O94" s="5"/>
       <c r="P94" s="5"/>
     </row>
-    <row r="95" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="B95" s="9" t="s">
         <v>271</v>
       </c>
@@ -5248,7 +5283,7 @@
       <c r="O95" s="5"/>
       <c r="P95" s="5"/>
     </row>
-    <row r="96" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="B96" s="9" t="s">
         <v>271</v>
       </c>
@@ -5279,7 +5314,7 @@
       <c r="O96" s="5"/>
       <c r="P96" s="5"/>
     </row>
-    <row r="97" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="B97" s="9" t="s">
         <v>271</v>
       </c>
@@ -5310,7 +5345,7 @@
       <c r="O97" s="5"/>
       <c r="P97" s="5"/>
     </row>
-    <row r="98" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="B98" s="9" t="s">
         <v>271</v>
       </c>
@@ -5341,7 +5376,7 @@
       <c r="O98" s="5"/>
       <c r="P98" s="5"/>
     </row>
-    <row r="99" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="B99" s="9" t="s">
         <v>271</v>
       </c>
@@ -5372,7 +5407,7 @@
       <c r="O99" s="5"/>
       <c r="P99" s="5"/>
     </row>
-    <row r="100" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:20" x14ac:dyDescent="0.2">
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
       <c r="J100" s="5"/>

</xml_diff>

<commit_message>
Cosmetic changes on the iApply CCBS Interfaces excel file
</commit_message>
<xml_diff>
--- a/iApply_CCBS_Interfaces.xlsx
+++ b/iApply_CCBS_Interfaces.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79945079-9C8D-463B-B6B4-47BEAC4F1060}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511F0AE3-BACF-445D-B41E-F4C907302AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11025" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CCBS_API_CALLS" sheetId="5" r:id="rId1"/>
@@ -1186,7 +1186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1224,9 +1224,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
@@ -1267,6 +1264,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1557,6 +1563,11 @@
       </filters>
     </filterColumn>
   </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:P93">
+    <sortCondition ref="F3:F99"/>
+    <sortCondition ref="G3:G99"/>
+    <sortCondition ref="C3:C99"/>
+  </sortState>
   <tableColumns count="15">
     <tableColumn id="5" xr3:uid="{439C2326-B5B7-468F-998C-E1E2D33178F2}" name="Color" dataDxfId="14"/>
     <tableColumn id="7" xr3:uid="{E6F3ECB4-BA57-46DA-9083-F5256AC0F6BA}" name="Group" dataDxfId="13"/>
@@ -1579,9 +1590,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1619,9 +1630,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1654,26 +1665,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1706,26 +1700,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1906,44 +1883,44 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.5703125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.28515625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" style="2"/>
-    <col min="18" max="18" width="14.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" style="2"/>
-    <col min="20" max="20" width="14.42578125" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="1.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="28.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.5546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.33203125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="2"/>
+    <col min="18" max="18" width="14.44140625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" style="2"/>
+    <col min="20" max="20" width="14.44140625" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:16" ht="8.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
-      <c r="C1" s="17">
+      <c r="C1" s="16">
         <v>3</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="F1" s="17">
-        <v>1</v>
-      </c>
-      <c r="G1" s="17">
+      <c r="D1" s="17"/>
+      <c r="F1" s="16">
+        <v>1</v>
+      </c>
+      <c r="G1" s="16">
         <v>2</v>
       </c>
       <c r="H1" s="1"/>
@@ -1953,14 +1930,14 @@
       <c r="M1" s="3"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="2:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>272</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>280</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -2000,131 +1977,135 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" ht="48" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>299</v>
-      </c>
-      <c r="E3" s="15"/>
+        <v>207</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>309</v>
+      </c>
       <c r="F3" s="4">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>287</v>
+        <v>120</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>288</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>268</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="J3" s="5"/>
       <c r="K3" s="4">
         <v>1</v>
       </c>
-      <c r="L3" s="15" t="s">
-        <v>1</v>
+      <c r="L3" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="E4" s="15"/>
+        <v>207</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>309</v>
+      </c>
       <c r="F4" s="4">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="H4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>266</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="J4" s="5"/>
       <c r="K4" s="4">
         <v>1</v>
       </c>
-      <c r="L4" s="15" t="s">
-        <v>0</v>
+      <c r="L4" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" ht="36" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>299</v>
-      </c>
-      <c r="E5" s="15"/>
+        <v>207</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>309</v>
+      </c>
       <c r="F5" s="4">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="H5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="K5" s="4">
-        <v>1</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="N5" s="5"/>
+        <v>314</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>278</v>
+      </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="2:16" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>270</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="5"/>
       <c r="F6" s="4">
         <v>100</v>
@@ -2152,246 +2133,252 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="2:16" ht="36" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" ht="48" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="15"/>
+      <c r="E7" s="14" t="s">
+        <v>308</v>
+      </c>
       <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="K7" s="4">
         <v>4</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="K7" s="4">
+      <c r="L7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="15" t="s">
-        <v>0</v>
-      </c>
       <c r="M7" s="5" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="2:16" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" ht="48" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="E8" s="15"/>
+        <v>206</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>308</v>
+      </c>
       <c r="F8" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="H8" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>192</v>
+        <v>21</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="K8" s="4">
-        <v>1</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="N8" s="5"/>
+        <v>306</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>295</v>
+      </c>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="2:16" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="14" t="s">
+        <v>308</v>
+      </c>
       <c r="F9" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>287</v>
+        <v>102</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>288</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K9" s="4">
-        <v>3</v>
-      </c>
-      <c r="L9" s="15" t="s">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L9" s="14"/>
       <c r="M9" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>293</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>298</v>
-      </c>
-      <c r="E10" s="15"/>
+        <v>207</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>309</v>
+      </c>
       <c r="F10" s="4">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>287</v>
+        <v>115</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>292</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="4">
         <v>1</v>
       </c>
-      <c r="L10" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>331</v>
+      <c r="L10" s="15"/>
+      <c r="M10" s="5" t="s">
+        <v>223</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="2:16" ht="36" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E11" s="15"/>
+        <v>205</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>319</v>
+      </c>
       <c r="F11" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>289</v>
+        <v>137</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>287</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="4">
         <v>1</v>
       </c>
-      <c r="L11" s="15" t="s">
-        <v>2</v>
+      <c r="L11" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="2:16" ht="36" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="E12" s="15"/>
+        <v>205</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>319</v>
+      </c>
       <c r="F12" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>289</v>
+        <v>138</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>288</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="4">
         <v>1</v>
       </c>
-      <c r="L12" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>325</v>
+      <c r="L12" s="15"/>
+      <c r="M12" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>270</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D13" s="20"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="5"/>
       <c r="F13" s="4">
         <v>100</v>
@@ -2417,51 +2404,55 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="E14" s="15"/>
+        <v>205</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>319</v>
+      </c>
       <c r="F14" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="H14" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J14" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>265</v>
+      </c>
       <c r="K14" s="4">
         <v>1</v>
       </c>
-      <c r="L14" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="14" t="s">
-        <v>326</v>
+      <c r="L14" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>226</v>
       </c>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>270</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D15" s="20"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="5"/>
       <c r="F15" s="4">
         <v>100</v>
@@ -2487,88 +2478,94 @@
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="E16" s="15"/>
+        <v>205</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>319</v>
+      </c>
       <c r="F16" s="4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H16" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>260</v>
+      </c>
       <c r="K16" s="4">
         <v>1</v>
       </c>
-      <c r="L16" s="15" t="s">
-        <v>2</v>
-      </c>
+      <c r="L16" s="15"/>
       <c r="M16" s="5" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:16" ht="36" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="E17" s="15"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="4">
         <v>4</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>290</v>
+        <v>103</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>287</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>254</v>
+      </c>
       <c r="K17" s="4">
-        <v>1</v>
-      </c>
-      <c r="L17" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>0</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="N17" s="5"/>
+        <v>310</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="D18" s="20"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="5"/>
       <c r="F18" s="4">
         <v>999</v>
@@ -2592,14 +2589,14 @@
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
-    <row r="19" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="D19" s="20"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="5"/>
       <c r="F19" s="4">
         <v>999</v>
@@ -2623,14 +2620,14 @@
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
     </row>
-    <row r="20" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="D20" s="20"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="5"/>
       <c r="F20" s="4">
         <v>999</v>
@@ -2654,14 +2651,14 @@
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="D21" s="20"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="5"/>
       <c r="F21" s="4">
         <v>999</v>
@@ -2685,14 +2682,14 @@
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
     </row>
-    <row r="22" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="D22" s="20"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="5"/>
       <c r="F22" s="4">
         <v>999</v>
@@ -2716,14 +2713,14 @@
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="D23" s="20"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="5"/>
       <c r="F23" s="4">
         <v>999</v>
@@ -2747,14 +2744,14 @@
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="D24" s="20"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="5"/>
       <c r="F24" s="4">
         <v>999</v>
@@ -2778,14 +2775,14 @@
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="D25" s="20"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="5"/>
       <c r="F25" s="4">
         <v>999</v>
@@ -2809,14 +2806,14 @@
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="D26" s="20"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="5"/>
       <c r="F26" s="4">
         <v>999</v>
@@ -2840,14 +2837,14 @@
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="D27" s="20"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="5"/>
       <c r="F27" s="4">
         <v>999</v>
@@ -2871,14 +2868,14 @@
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
     </row>
-    <row r="28" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="D28" s="20"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="5"/>
       <c r="F28" s="4">
         <v>999</v>
@@ -2902,759 +2899,743 @@
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
     </row>
-    <row r="29" spans="2:16" ht="36" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:16" ht="36" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="E29" s="15"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="4">
         <v>4</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>289</v>
+        <v>107</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>287</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="J29" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>254</v>
+      </c>
       <c r="K29" s="4">
-        <v>1</v>
-      </c>
-      <c r="L29" s="15" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="L29" s="14" t="s">
+        <v>0</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="N29" s="5"/>
+        <v>311</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>293</v>
+      </c>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
     </row>
-    <row r="30" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="E30" s="15"/>
+      <c r="E30" s="14"/>
       <c r="F30" s="4">
         <v>4</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>290</v>
+        <v>116</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>289</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="4">
         <v>1</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="L30" s="14" t="s">
         <v>2</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="E31" s="15"/>
+        <v>206</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="E31" s="14"/>
       <c r="F31" s="4">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>287</v>
+        <v>112</v>
+      </c>
+      <c r="H31" s="28" t="s">
+        <v>290</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="4">
         <v>1</v>
       </c>
-      <c r="L31" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="M31" s="14" t="s">
-        <v>333</v>
+      <c r="L31" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>220</v>
       </c>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
     </row>
-    <row r="32" spans="2:16" ht="60" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:16" ht="36" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>309</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="E32" s="14"/>
       <c r="F32" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>288</v>
+        <v>117</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>289</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="4">
         <v>1</v>
       </c>
-      <c r="L32" s="15" t="s">
-        <v>3</v>
+      <c r="L32" s="14" t="s">
+        <v>1</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="E33" s="15"/>
+        <v>206</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="E33" s="14"/>
       <c r="F33" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>292</v>
+        <v>111</v>
+      </c>
+      <c r="H33" s="28" t="s">
+        <v>290</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="4">
         <v>1</v>
       </c>
-      <c r="L33" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="M33" s="14" t="s">
-        <v>337</v>
+      <c r="L33" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>219</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
     </row>
-    <row r="34" spans="2:16" s="27" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="B34" s="6" t="s">
+    <row r="34" spans="2:16" s="26" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="B34" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="F34" s="4">
-        <v>1</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H34" s="4" t="s">
+      <c r="C34" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="E34" s="24"/>
+      <c r="F34" s="25">
+        <v>4</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H34" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="I34" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J34" s="5"/>
-      <c r="K34" s="4">
-        <v>1</v>
-      </c>
-      <c r="L34" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-    </row>
-    <row r="35" spans="2:16" ht="36" x14ac:dyDescent="0.2">
-      <c r="B35" s="6" t="s">
+      <c r="I34" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="K34" s="25">
+        <v>1</v>
+      </c>
+      <c r="L34" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="M34" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+    </row>
+    <row r="35" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+      <c r="B35" s="27" t="s">
         <v>269</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>309</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="E35" s="14"/>
       <c r="F35" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="H35" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H35" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>259</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="J35" s="5"/>
       <c r="K35" s="4">
         <v>2</v>
       </c>
-      <c r="L35" s="15" t="s">
-        <v>3</v>
+      <c r="L35" s="14" t="s">
+        <v>0</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="N35" s="5" t="s">
-        <v>278</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
     </row>
-    <row r="36" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:16" ht="48" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>319</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="E36" s="14"/>
       <c r="F36" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="H36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H36" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="J36" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="K36" s="4">
-        <v>1</v>
-      </c>
-      <c r="L36" s="15" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="L36" s="14" t="s">
+        <v>1</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="N36" s="5"/>
+        <v>312</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>296</v>
+      </c>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
     </row>
-    <row r="37" spans="2:16" ht="36" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:16" ht="36" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>319</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="E37" s="14"/>
       <c r="F37" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>288</v>
+        <v>105</v>
+      </c>
+      <c r="H37" s="28" t="s">
+        <v>287</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J37" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="K37" s="4">
-        <v>1</v>
-      </c>
-      <c r="L37" s="16"/>
+        <v>3</v>
+      </c>
+      <c r="L37" s="14" t="s">
+        <v>1</v>
+      </c>
       <c r="M37" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="N37" s="5"/>
+        <v>313</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
-    <row r="38" spans="2:16" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D38" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>319</v>
-      </c>
+      <c r="D38" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="E38" s="14"/>
       <c r="F38" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="H38" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="H38" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>52</v>
+        <v>192</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K38" s="4">
         <v>1</v>
       </c>
-      <c r="L38" s="15" t="s">
-        <v>3</v>
+      <c r="L38" s="14" t="s">
+        <v>0</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
     </row>
-    <row r="39" spans="2:16" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:16" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D39" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>319</v>
-      </c>
+      <c r="D39" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="E39" s="14"/>
       <c r="F39" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>287</v>
+        <v>124</v>
+      </c>
+      <c r="H39" s="28" t="s">
+        <v>292</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>260</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="J39" s="5"/>
       <c r="K39" s="4">
         <v>1</v>
       </c>
-      <c r="L39" s="16"/>
-      <c r="M39" s="5" t="s">
-        <v>227</v>
+      <c r="L39" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M39" s="30" t="s">
+        <v>337</v>
       </c>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
     </row>
-    <row r="40" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="E40" s="15"/>
+        <v>205</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="E40" s="14"/>
       <c r="F40" s="4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>287</v>
+        <v>123</v>
+      </c>
+      <c r="H40" s="28" t="s">
+        <v>292</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="4">
         <v>1</v>
       </c>
-      <c r="L40" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="M40" s="14" t="s">
-        <v>320</v>
+      <c r="L40" s="15"/>
+      <c r="M40" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
     </row>
-    <row r="41" spans="2:16" ht="24" x14ac:dyDescent="0.2">
-      <c r="B41" s="22" t="s">
+    <row r="41" spans="2:16" ht="24" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C41" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="D41" s="24" t="s">
-        <v>282</v>
-      </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="26">
-        <v>4</v>
-      </c>
-      <c r="G41" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="H41" s="26" t="s">
+      <c r="C41" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="E41" s="14"/>
+      <c r="F41" s="4">
+        <v>6</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41" s="28" t="s">
         <v>287</v>
       </c>
-      <c r="I41" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J41" s="23" t="s">
-        <v>258</v>
-      </c>
-      <c r="K41" s="26">
-        <v>1</v>
-      </c>
-      <c r="L41" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="M41" s="23" t="s">
-        <v>222</v>
-      </c>
-      <c r="N41" s="23"/>
-      <c r="O41" s="23"/>
-      <c r="P41" s="23"/>
-    </row>
-    <row r="42" spans="2:16" ht="48" x14ac:dyDescent="0.2">
+      <c r="I41" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="K41" s="4">
+        <v>1</v>
+      </c>
+      <c r="L41" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+    </row>
+    <row r="42" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>308</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="E42" s="14"/>
       <c r="F42" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H42" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H42" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>256</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="J42" s="5"/>
       <c r="K42" s="4">
-        <v>4</v>
-      </c>
-      <c r="L42" s="15" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="L42" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="N42" s="5" t="s">
-        <v>294</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="N42" s="5"/>
       <c r="O42" s="5"/>
       <c r="P42" s="5"/>
     </row>
-    <row r="43" spans="2:16" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>308</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" s="14"/>
       <c r="F43" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H43" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="H43" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>257</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="J43" s="5"/>
       <c r="K43" s="4">
-        <v>4</v>
-      </c>
-      <c r="L43" s="15" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="L43" s="14" t="s">
+        <v>0</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="N43" s="5" t="s">
-        <v>295</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="N43" s="5"/>
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
     </row>
-    <row r="44" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>298</v>
-      </c>
-      <c r="E44" s="15"/>
+        <v>212</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="E44" s="14"/>
       <c r="F44" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>292</v>
+        <v>182</v>
+      </c>
+      <c r="H44" s="28" t="s">
+        <v>289</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="4">
         <v>1</v>
       </c>
-      <c r="L44" s="16"/>
-      <c r="M44" s="5" t="s">
-        <v>237</v>
+      <c r="L44" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M44" s="30" t="s">
+        <v>325</v>
       </c>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
     </row>
-    <row r="45" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D45" s="20" t="s">
+      <c r="D45" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="E45" s="15"/>
+      <c r="E45" s="14"/>
       <c r="F45" s="4">
         <v>10</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="H45" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H45" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="4">
         <v>1</v>
       </c>
-      <c r="L45" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="M45" s="14" t="s">
-        <v>321</v>
+      <c r="L45" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M45" s="30" t="s">
+        <v>326</v>
       </c>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
     </row>
-    <row r="46" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="E46" s="15"/>
+        <v>212</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="E46" s="14"/>
       <c r="F46" s="4">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="H46" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="H46" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>261</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="J46" s="5"/>
       <c r="K46" s="4">
         <v>1</v>
       </c>
-      <c r="L46" s="15" t="s">
+      <c r="L46" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="M46" s="14" t="s">
-        <v>324</v>
+      <c r="M46" s="30" t="s">
+        <v>320</v>
       </c>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
     </row>
-    <row r="47" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E47" s="15"/>
+        <v>212</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="E47" s="14"/>
       <c r="F47" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="H47" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="H47" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>304</v>
+        <v>90</v>
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="4">
         <v>1</v>
       </c>
-      <c r="L47" s="15" t="s">
+      <c r="L47" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="M47" s="5" t="s">
-        <v>225</v>
+      <c r="M47" s="30" t="s">
+        <v>321</v>
       </c>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
     </row>
-    <row r="48" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D48" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="E48" s="15"/>
+      <c r="E48" s="14"/>
       <c r="F48" s="4">
         <v>10</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="H48" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I48" s="5" t="s">
@@ -3666,439 +3647,437 @@
       <c r="K48" s="4">
         <v>1</v>
       </c>
-      <c r="L48" s="15" t="s">
+      <c r="L48" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="M48" s="14" t="s">
+      <c r="M48" s="30" t="s">
         <v>322</v>
       </c>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="E49" s="15"/>
+        <v>212</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="E49" s="14"/>
       <c r="F49" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="H49" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="H49" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="J49" s="5"/>
       <c r="K49" s="4">
         <v>1</v>
       </c>
-      <c r="L49" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="M49" s="14" t="s">
-        <v>334</v>
+      <c r="L49" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M49" s="30" t="s">
+        <v>327</v>
       </c>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
     </row>
-    <row r="50" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="D50" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="E50" s="15"/>
+      <c r="E50" s="14"/>
       <c r="F50" s="4">
         <v>10</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="H50" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="H50" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J50" s="5"/>
       <c r="K50" s="4">
         <v>1</v>
       </c>
-      <c r="L50" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="M50" s="14" t="s">
-        <v>327</v>
+      <c r="L50" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M50" s="30" t="s">
+        <v>323</v>
       </c>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
     </row>
-    <row r="51" spans="2:16" ht="36" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D51" s="20" t="s">
+      <c r="D51" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="E51" s="15"/>
+      <c r="E51" s="14"/>
       <c r="F51" s="4">
         <v>12</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="H51" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H51" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="K51" s="4">
         <v>1</v>
       </c>
-      <c r="L51" s="15" t="s">
-        <v>3</v>
+      <c r="L51" s="14" t="s">
+        <v>0</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
     </row>
-    <row r="52" spans="2:16" ht="36" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="D52" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="E52" s="15"/>
+        <v>100</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="E52" s="14"/>
       <c r="F52" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>289</v>
+        <v>128</v>
+      </c>
+      <c r="H52" s="28" t="s">
+        <v>287</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>291</v>
+        <v>39</v>
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="4">
         <v>1</v>
       </c>
-      <c r="L52" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="M52" s="14" t="s">
-        <v>328</v>
+      <c r="L52" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>240</v>
       </c>
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
       <c r="P52" s="5"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B53" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>299</v>
-      </c>
-      <c r="E53" s="15"/>
+        <v>100</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="E53" s="14"/>
       <c r="F53" s="4">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="H53" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H53" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>194</v>
+        <v>40</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="K53" s="4">
         <v>1</v>
       </c>
-      <c r="L53" s="15" t="s">
+      <c r="L53" s="14" t="s">
         <v>3</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
       <c r="P53" s="5"/>
     </row>
-    <row r="54" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="E54" s="15"/>
+        <v>100</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="E54" s="14"/>
       <c r="F54" s="4">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="H54" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H54" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="J54" s="5"/>
       <c r="K54" s="4">
         <v>1</v>
       </c>
-      <c r="L54" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="M54" s="14" t="s">
-        <v>335</v>
+      <c r="L54" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="N54" s="5"/>
       <c r="O54" s="5"/>
       <c r="P54" s="5"/>
     </row>
-    <row r="55" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D55" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="E55" s="15"/>
+        <v>208</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="E55" s="14"/>
       <c r="F55" s="4">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H55" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H55" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="K55" s="4">
         <v>1</v>
       </c>
-      <c r="L55" s="15" t="s">
+      <c r="L55" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="M55" s="5" t="s">
-        <v>230</v>
+      <c r="M55" s="30" t="s">
+        <v>324</v>
       </c>
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
     </row>
-    <row r="56" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D56" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E56" s="15"/>
+        <v>208</v>
+      </c>
+      <c r="D56" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="E56" s="14"/>
       <c r="F56" s="4">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>287</v>
+        <v>132</v>
+      </c>
+      <c r="H56" s="28" t="s">
+        <v>289</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>53</v>
+        <v>291</v>
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="4">
         <v>1</v>
       </c>
-      <c r="L56" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="M56" s="5" t="s">
-        <v>228</v>
+      <c r="L56" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M56" s="30" t="s">
+        <v>328</v>
       </c>
       <c r="N56" s="5"/>
       <c r="O56" s="5"/>
       <c r="P56" s="5"/>
     </row>
-    <row r="57" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B57" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E57" s="15" t="s">
-        <v>308</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="E57" s="14"/>
       <c r="F57" s="4">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>288</v>
+        <v>131</v>
+      </c>
+      <c r="H57" s="28" t="s">
+        <v>287</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J57" s="5" t="s">
-        <v>253</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="J57" s="5"/>
       <c r="K57" s="4">
         <v>1</v>
       </c>
-      <c r="L57" s="15"/>
-      <c r="M57" s="5" t="s">
-        <v>215</v>
+      <c r="L57" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M57" s="30" t="s">
+        <v>329</v>
       </c>
       <c r="N57" s="5"/>
       <c r="O57" s="5"/>
       <c r="P57" s="5"/>
     </row>
-    <row r="58" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>309</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="E58" s="14"/>
       <c r="F58" s="4">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>292</v>
+        <v>133</v>
+      </c>
+      <c r="H58" s="28" t="s">
+        <v>287</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J58" s="5"/>
       <c r="K58" s="4">
         <v>1</v>
       </c>
-      <c r="L58" s="16"/>
-      <c r="M58" s="5" t="s">
-        <v>223</v>
+      <c r="L58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M58" s="30" t="s">
+        <v>330</v>
       </c>
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
       <c r="P58" s="5"/>
     </row>
-    <row r="59" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="E59" s="15"/>
+        <v>204</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="E59" s="14"/>
       <c r="F59" s="4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="H59" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H59" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="J59" s="5"/>
       <c r="K59" s="4">
         <v>1</v>
       </c>
-      <c r="L59" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M59" s="14" t="s">
-        <v>323</v>
+      <c r="L59" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M59" s="30" t="s">
+        <v>331</v>
       </c>
       <c r="N59" s="5"/>
       <c r="O59" s="5"/>
       <c r="P59" s="5"/>
     </row>
-    <row r="60" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D60" s="20"/>
+      <c r="D60" s="19"/>
       <c r="E60" s="5"/>
       <c r="F60" s="4">
         <v>999</v>
@@ -4122,14 +4101,14 @@
       <c r="O60" s="5"/>
       <c r="P60" s="5"/>
     </row>
-    <row r="61" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D61" s="20"/>
+      <c r="D61" s="19"/>
       <c r="E61" s="5"/>
       <c r="F61" s="4">
         <v>999</v>
@@ -4153,14 +4132,14 @@
       <c r="O61" s="5"/>
       <c r="P61" s="5"/>
     </row>
-    <row r="62" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D62" s="20"/>
+      <c r="D62" s="19"/>
       <c r="E62" s="5"/>
       <c r="F62" s="4">
         <v>999</v>
@@ -4184,14 +4163,14 @@
       <c r="O62" s="5"/>
       <c r="P62" s="5"/>
     </row>
-    <row r="63" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D63" s="20"/>
+      <c r="D63" s="19"/>
       <c r="E63" s="5"/>
       <c r="F63" s="4">
         <v>999</v>
@@ -4215,14 +4194,14 @@
       <c r="O63" s="5"/>
       <c r="P63" s="5"/>
     </row>
-    <row r="64" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D64" s="20"/>
+      <c r="D64" s="19"/>
       <c r="E64" s="5"/>
       <c r="F64" s="4">
         <v>999</v>
@@ -4246,14 +4225,14 @@
       <c r="O64" s="5"/>
       <c r="P64" s="5"/>
     </row>
-    <row r="65" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D65" s="20"/>
+      <c r="D65" s="19"/>
       <c r="E65" s="5"/>
       <c r="F65" s="4">
         <v>999</v>
@@ -4275,14 +4254,14 @@
       <c r="O65" s="5"/>
       <c r="P65" s="5"/>
     </row>
-    <row r="66" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D66" s="20"/>
+      <c r="D66" s="19"/>
       <c r="E66" s="5"/>
       <c r="F66" s="4">
         <v>999</v>
@@ -4306,14 +4285,14 @@
       <c r="O66" s="5"/>
       <c r="P66" s="5"/>
     </row>
-    <row r="67" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D67" s="20"/>
+      <c r="D67" s="19"/>
       <c r="E67" s="5"/>
       <c r="F67" s="4">
         <v>999</v>
@@ -4337,88 +4316,88 @@
       <c r="O67" s="5"/>
       <c r="P67" s="5"/>
     </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B68" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D68" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="E68" s="15"/>
+        <v>204</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="E68" s="14"/>
       <c r="F68" s="4">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="H68" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H68" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="J68" s="5"/>
       <c r="K68" s="4">
         <v>1</v>
       </c>
-      <c r="L68" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M68" s="5" t="s">
-        <v>239</v>
+      <c r="L68" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M68" s="30" t="s">
+        <v>332</v>
       </c>
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
       <c r="P68" s="5"/>
     </row>
-    <row r="69" spans="2:16" ht="24" x14ac:dyDescent="0.2">
-      <c r="B69" s="28" t="s">
+    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B69" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D69" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E69" s="15"/>
+        <v>211</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="E69" s="14"/>
       <c r="F69" s="4">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="H69" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H69" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="J69" s="5"/>
       <c r="K69" s="4">
+        <v>1</v>
+      </c>
+      <c r="L69" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="L69" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="M69" s="5" t="s">
-        <v>216</v>
+      <c r="M69" s="30" t="s">
+        <v>333</v>
       </c>
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
       <c r="P69" s="5"/>
     </row>
-    <row r="70" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D70" s="20"/>
+      <c r="D70" s="19"/>
       <c r="E70" s="5"/>
       <c r="F70" s="4">
         <v>999</v>
@@ -4444,14 +4423,14 @@
       <c r="O70" s="5"/>
       <c r="P70" s="5"/>
     </row>
-    <row r="71" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D71" s="20"/>
+      <c r="D71" s="19"/>
       <c r="E71" s="5"/>
       <c r="F71" s="4">
         <v>999</v>
@@ -4477,14 +4456,14 @@
       <c r="O71" s="5"/>
       <c r="P71" s="5"/>
     </row>
-    <row r="72" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D72" s="20"/>
+      <c r="D72" s="19"/>
       <c r="E72" s="5"/>
       <c r="F72" s="4">
         <v>999</v>
@@ -4508,14 +4487,14 @@
       <c r="O72" s="5"/>
       <c r="P72" s="5"/>
     </row>
-    <row r="73" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D73" s="20"/>
+      <c r="D73" s="19"/>
       <c r="E73" s="5"/>
       <c r="F73" s="4">
         <v>999</v>
@@ -4539,14 +4518,14 @@
       <c r="O73" s="5"/>
       <c r="P73" s="5"/>
     </row>
-    <row r="74" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D74" s="20"/>
+      <c r="D74" s="19"/>
       <c r="E74" s="5"/>
       <c r="F74" s="4">
         <v>999</v>
@@ -4572,14 +4551,14 @@
       <c r="O74" s="5"/>
       <c r="P74" s="5"/>
     </row>
-    <row r="75" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D75" s="20"/>
+      <c r="D75" s="19"/>
       <c r="E75" s="5"/>
       <c r="F75" s="4">
         <v>999</v>
@@ -4605,14 +4584,14 @@
       <c r="O75" s="5"/>
       <c r="P75" s="5"/>
     </row>
-    <row r="76" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D76" s="20"/>
+      <c r="D76" s="19"/>
       <c r="E76" s="5"/>
       <c r="F76" s="4">
         <v>999</v>
@@ -4638,14 +4617,14 @@
       <c r="O76" s="5"/>
       <c r="P76" s="5"/>
     </row>
-    <row r="77" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D77" s="20"/>
+      <c r="D77" s="19"/>
       <c r="E77" s="5"/>
       <c r="F77" s="4">
         <v>999</v>
@@ -4669,14 +4648,14 @@
       <c r="O77" s="5"/>
       <c r="P77" s="5"/>
     </row>
-    <row r="78" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D78" s="20"/>
+      <c r="D78" s="19"/>
       <c r="E78" s="5"/>
       <c r="F78" s="4">
         <v>999</v>
@@ -4700,14 +4679,14 @@
       <c r="O78" s="5"/>
       <c r="P78" s="5"/>
     </row>
-    <row r="79" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D79" s="20"/>
+      <c r="D79" s="19"/>
       <c r="E79" s="5"/>
       <c r="F79" s="4">
         <v>999</v>
@@ -4733,14 +4712,14 @@
       <c r="O79" s="5"/>
       <c r="P79" s="5"/>
     </row>
-    <row r="80" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D80" s="20"/>
+      <c r="D80" s="19"/>
       <c r="E80" s="5"/>
       <c r="F80" s="4">
         <v>999</v>
@@ -4766,14 +4745,14 @@
       <c r="O80" s="5"/>
       <c r="P80" s="5"/>
     </row>
-    <row r="81" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D81" s="20"/>
+      <c r="D81" s="19"/>
       <c r="E81" s="5"/>
       <c r="F81" s="4">
         <v>999</v>
@@ -4799,14 +4778,14 @@
       <c r="O81" s="5"/>
       <c r="P81" s="5"/>
     </row>
-    <row r="82" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D82" s="20"/>
+      <c r="D82" s="19"/>
       <c r="E82" s="5"/>
       <c r="F82" s="4">
         <v>999</v>
@@ -4830,14 +4809,14 @@
       <c r="O82" s="5"/>
       <c r="P82" s="5"/>
     </row>
-    <row r="83" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D83" s="20"/>
+      <c r="D83" s="19"/>
       <c r="E83" s="5"/>
       <c r="F83" s="4">
         <v>999</v>
@@ -4861,14 +4840,14 @@
       <c r="O83" s="5"/>
       <c r="P83" s="5"/>
     </row>
-    <row r="84" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B84" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D84" s="20"/>
+      <c r="D84" s="19"/>
       <c r="E84" s="5"/>
       <c r="F84" s="4">
         <v>999</v>
@@ -4894,14 +4873,14 @@
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
     </row>
-    <row r="85" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D85" s="20"/>
+      <c r="D85" s="19"/>
       <c r="E85" s="5"/>
       <c r="F85" s="4">
         <v>999</v>
@@ -4927,14 +4906,14 @@
       <c r="O85" s="5"/>
       <c r="P85" s="5"/>
     </row>
-    <row r="86" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D86" s="20"/>
+      <c r="D86" s="19"/>
       <c r="E86" s="5"/>
       <c r="F86" s="4">
         <v>999</v>
@@ -4960,14 +4939,14 @@
       <c r="O86" s="5"/>
       <c r="P86" s="5"/>
     </row>
-    <row r="87" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D87" s="20"/>
+      <c r="D87" s="19"/>
       <c r="E87" s="5"/>
       <c r="F87" s="4">
         <v>999</v>
@@ -4991,244 +4970,242 @@
       <c r="O87" s="5"/>
       <c r="P87" s="5"/>
     </row>
-    <row r="88" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B88" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="D88" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="E88" s="15"/>
+        <v>211</v>
+      </c>
+      <c r="D88" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="E88" s="14"/>
       <c r="F88" s="4">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="H88" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="H88" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I88" s="5" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="J88" s="5"/>
       <c r="K88" s="4">
         <v>1</v>
       </c>
-      <c r="L88" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M88" s="14" t="s">
-        <v>329</v>
+      <c r="L88" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M88" s="30" t="s">
+        <v>334</v>
       </c>
       <c r="N88" s="5"/>
       <c r="O88" s="5"/>
       <c r="P88" s="5"/>
     </row>
-    <row r="89" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B89" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="D89" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="E89" s="15"/>
+        <v>211</v>
+      </c>
+      <c r="D89" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="E89" s="14"/>
       <c r="F89" s="4">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H89" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H89" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="J89" s="5"/>
       <c r="K89" s="4">
         <v>1</v>
       </c>
-      <c r="L89" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="M89" s="14" t="s">
-        <v>330</v>
+      <c r="L89" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M89" s="30" t="s">
+        <v>335</v>
       </c>
       <c r="N89" s="5"/>
       <c r="O89" s="5"/>
       <c r="P89" s="5"/>
     </row>
-    <row r="90" spans="2:16" ht="48" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B90" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D90" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E90" s="15"/>
+        <v>211</v>
+      </c>
+      <c r="D90" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="E90" s="14"/>
       <c r="F90" s="4">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H90" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="H90" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J90" s="5" t="s">
-        <v>255</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="J90" s="5"/>
       <c r="K90" s="4">
-        <v>4</v>
-      </c>
-      <c r="L90" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M90" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="N90" s="5" t="s">
-        <v>296</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L90" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M90" s="30" t="s">
+        <v>336</v>
+      </c>
+      <c r="N90" s="5"/>
       <c r="O90" s="5"/>
       <c r="P90" s="5"/>
     </row>
-    <row r="91" spans="2:16" ht="36" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B91" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E91" s="15"/>
+        <v>205</v>
+      </c>
+      <c r="D91" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="E91" s="14"/>
       <c r="F91" s="4">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="H91" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H91" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="K91" s="4">
-        <v>3</v>
-      </c>
-      <c r="L91" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L91" s="14" t="s">
         <v>1</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="N91" s="5" t="s">
-        <v>297</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="N91" s="5"/>
       <c r="O91" s="5"/>
       <c r="P91" s="5"/>
     </row>
-    <row r="92" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B92" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>298</v>
-      </c>
-      <c r="E92" s="15"/>
+        <v>205</v>
+      </c>
+      <c r="D92" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="E92" s="14"/>
       <c r="F92" s="4">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="H92" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H92" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I92" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J92" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>268</v>
+      </c>
       <c r="K92" s="4">
         <v>1</v>
       </c>
-      <c r="L92" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M92" s="14" t="s">
-        <v>332</v>
+      <c r="L92" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="M92" s="5" t="s">
+        <v>234</v>
       </c>
       <c r="N92" s="5"/>
       <c r="O92" s="5"/>
       <c r="P92" s="5"/>
     </row>
-    <row r="93" spans="2:16" ht="24" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B93" s="6" t="s">
         <v>269</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D93" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="E93" s="15"/>
+        <v>205</v>
+      </c>
+      <c r="D93" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="E93" s="14"/>
       <c r="F93" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="H93" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="H93" s="28" t="s">
         <v>287</v>
       </c>
       <c r="I93" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="J93" s="5"/>
+        <v>194</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>268</v>
+      </c>
       <c r="K93" s="4">
         <v>1</v>
       </c>
-      <c r="L93" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M93" s="14" t="s">
-        <v>336</v>
+      <c r="L93" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M93" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="N93" s="5"/>
       <c r="O93" s="5"/>
       <c r="P93" s="5"/>
     </row>
-    <row r="94" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B94" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D94" s="20"/>
+      <c r="D94" s="19"/>
       <c r="E94" s="5"/>
       <c r="F94" s="4">
         <v>999</v>
@@ -5252,14 +5229,14 @@
       <c r="O94" s="5"/>
       <c r="P94" s="5"/>
     </row>
-    <row r="95" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D95" s="20"/>
+      <c r="D95" s="19"/>
       <c r="E95" s="5"/>
       <c r="F95" s="4">
         <v>999</v>
@@ -5283,14 +5260,14 @@
       <c r="O95" s="5"/>
       <c r="P95" s="5"/>
     </row>
-    <row r="96" spans="2:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B96" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D96" s="20"/>
+      <c r="D96" s="19"/>
       <c r="E96" s="5"/>
       <c r="F96" s="4">
         <v>999</v>
@@ -5314,14 +5291,14 @@
       <c r="O96" s="5"/>
       <c r="P96" s="5"/>
     </row>
-    <row r="97" spans="2:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B97" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D97" s="20"/>
+      <c r="D97" s="19"/>
       <c r="E97" s="5"/>
       <c r="F97" s="4">
         <v>999</v>
@@ -5345,14 +5322,14 @@
       <c r="O97" s="5"/>
       <c r="P97" s="5"/>
     </row>
-    <row r="98" spans="2:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B98" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D98" s="20"/>
+      <c r="D98" s="19"/>
       <c r="E98" s="5"/>
       <c r="F98" s="4">
         <v>999</v>
@@ -5376,14 +5353,14 @@
       <c r="O98" s="5"/>
       <c r="P98" s="5"/>
     </row>
-    <row r="99" spans="2:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B99" s="9" t="s">
         <v>271</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D99" s="20"/>
+      <c r="D99" s="19"/>
       <c r="E99" s="5"/>
       <c r="F99" s="4">
         <v>999</v>
@@ -5407,7 +5384,7 @@
       <c r="O99" s="5"/>
       <c r="P99" s="5"/>
     </row>
-    <row r="100" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
       <c r="J100" s="5"/>

</xml_diff>

<commit_message>
Minor modifications, template API C# application
</commit_message>
<xml_diff>
--- a/iApply_CCBS_Interfaces.xlsx
+++ b/iApply_CCBS_Interfaces.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511F0AE3-BACF-445D-B41E-F4C907302AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4451C0B7-A9DF-4DFE-8F9C-2CBA52BB3080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -659,9 +659,6 @@
     <t>Collateral General (Vehicles, Deposits, Cash, Shares, Bonds)</t>
   </si>
   <si>
-    <t>Retrievedrawdown</t>
-  </si>
-  <si>
     <t>Customer_Search.xlsx</t>
   </si>
   <si>
@@ -1050,6 +1047,9 @@
   </si>
   <si>
     <t>Exposures_DownloadDepts</t>
+  </si>
+  <si>
+    <t>RetrieveDrawDown</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1265,14 +1265,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1932,63 +1929,63 @@
     </row>
     <row r="2" spans="2:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>273</v>
-      </c>
       <c r="D2" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>281</v>
-      </c>
       <c r="F2" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>285</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>286</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K2" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>307</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="48" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>207</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
@@ -1997,7 +1994,7 @@
         <v>120</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>35</v>
@@ -2010,7 +2007,7 @@
         <v>3</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -2018,16 +2015,16 @@
     </row>
     <row r="4" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>207</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
@@ -2036,7 +2033,7 @@
         <v>118</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>45</v>
@@ -2049,7 +2046,7 @@
         <v>3</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -2057,16 +2054,16 @@
     </row>
     <row r="5" spans="2:16" ht="36" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>207</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
@@ -2075,13 +2072,13 @@
         <v>119</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>46</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K5" s="4">
         <v>2</v>
@@ -2090,17 +2087,17 @@
         <v>3</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>205</v>
@@ -2118,7 +2115,7 @@
         <v>192</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K6" s="4">
         <v>2</v>
@@ -2127,7 +2124,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -2135,16 +2132,16 @@
     </row>
     <row r="7" spans="2:16" ht="48" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
@@ -2153,13 +2150,13 @@
         <v>106</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K7" s="4">
         <v>4</v>
@@ -2168,26 +2165,26 @@
         <v>3</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="2:16" ht="48" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -2196,13 +2193,13 @@
         <v>108</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K8" s="4">
         <v>4</v>
@@ -2211,26 +2208,26 @@
         <v>3</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
     <row r="9" spans="2:16" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -2239,20 +2236,20 @@
         <v>102</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K9" s="4">
         <v>1</v>
       </c>
       <c r="L9" s="14"/>
       <c r="M9" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -2260,16 +2257,16 @@
     </row>
     <row r="10" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>207</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -2278,7 +2275,7 @@
         <v>115</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>43</v>
@@ -2289,7 +2286,7 @@
       </c>
       <c r="L10" s="15"/>
       <c r="M10" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -2297,16 +2294,16 @@
     </row>
     <row r="11" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F11" s="4">
         <v>2</v>
@@ -2315,7 +2312,7 @@
         <v>137</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>54</v>
@@ -2328,7 +2325,7 @@
         <v>11</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -2336,16 +2333,16 @@
     </row>
     <row r="12" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F12" s="4">
         <v>2</v>
@@ -2354,7 +2351,7 @@
         <v>138</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>55</v>
@@ -2365,7 +2362,7 @@
       </c>
       <c r="L12" s="15"/>
       <c r="M12" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
@@ -2373,7 +2370,7 @@
     </row>
     <row r="13" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>205</v>
@@ -2398,7 +2395,7 @@
         <v>13</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
@@ -2406,16 +2403,16 @@
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F14" s="4">
         <v>2</v>
@@ -2424,13 +2421,13 @@
         <v>134</v>
       </c>
       <c r="H14" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>52</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K14" s="4">
         <v>1</v>
@@ -2439,7 +2436,7 @@
         <v>3</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
@@ -2447,7 +2444,7 @@
     </row>
     <row r="15" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>205</v>
@@ -2472,7 +2469,7 @@
         <v>3</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -2480,16 +2477,16 @@
     </row>
     <row r="16" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F16" s="4">
         <v>2</v>
@@ -2498,20 +2495,20 @@
         <v>135</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>51</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K16" s="4">
         <v>1</v>
       </c>
       <c r="L16" s="15"/>
       <c r="M16" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
@@ -2519,13 +2516,13 @@
     </row>
     <row r="17" spans="2:16" ht="36" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="4">
@@ -2535,13 +2532,13 @@
         <v>103</v>
       </c>
       <c r="H17" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K17" s="4">
         <v>3</v>
@@ -2550,17 +2547,17 @@
         <v>0</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
     <row r="18" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>213</v>
@@ -2591,7 +2588,7 @@
     </row>
     <row r="19" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>213</v>
@@ -2622,7 +2619,7 @@
     </row>
     <row r="20" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>213</v>
@@ -2653,7 +2650,7 @@
     </row>
     <row r="21" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>213</v>
@@ -2684,7 +2681,7 @@
     </row>
     <row r="22" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>213</v>
@@ -2715,7 +2712,7 @@
     </row>
     <row r="23" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>213</v>
@@ -2746,7 +2743,7 @@
     </row>
     <row r="24" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>213</v>
@@ -2777,7 +2774,7 @@
     </row>
     <row r="25" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>213</v>
@@ -2808,7 +2805,7 @@
     </row>
     <row r="26" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>213</v>
@@ -2839,7 +2836,7 @@
     </row>
     <row r="27" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>213</v>
@@ -2870,7 +2867,7 @@
     </row>
     <row r="28" spans="2:16" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>213</v>
@@ -2901,13 +2898,13 @@
     </row>
     <row r="29" spans="2:16" ht="36" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="4">
@@ -2917,13 +2914,13 @@
         <v>107</v>
       </c>
       <c r="H29" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K29" s="4">
         <v>3</v>
@@ -2932,23 +2929,23 @@
         <v>0</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
     </row>
     <row r="30" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="4">
@@ -2958,7 +2955,7 @@
         <v>116</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>49</v>
@@ -2971,7 +2968,7 @@
         <v>2</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
@@ -2979,13 +2976,13 @@
     </row>
     <row r="31" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="4">
@@ -2995,7 +2992,7 @@
         <v>112</v>
       </c>
       <c r="H31" s="28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>28</v>
@@ -3008,7 +3005,7 @@
         <v>5</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
@@ -3016,13 +3013,13 @@
     </row>
     <row r="32" spans="2:16" ht="36" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="4">
@@ -3032,7 +3029,7 @@
         <v>117</v>
       </c>
       <c r="H32" s="28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>77</v>
@@ -3045,7 +3042,7 @@
         <v>1</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
@@ -3053,13 +3050,13 @@
     </row>
     <row r="33" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="4">
@@ -3069,7 +3066,7 @@
         <v>111</v>
       </c>
       <c r="H33" s="28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>27</v>
@@ -3082,7 +3079,7 @@
         <v>2</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
@@ -3090,13 +3087,13 @@
     </row>
     <row r="34" spans="2:16" s="26" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="B34" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C34" s="22" t="s">
         <v>206</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E34" s="24"/>
       <c r="F34" s="25">
@@ -3106,13 +3103,13 @@
         <v>109</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I34" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J34" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K34" s="25">
         <v>1</v>
@@ -3121,7 +3118,7 @@
         <v>4</v>
       </c>
       <c r="M34" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N34" s="22"/>
       <c r="O34" s="22"/>
@@ -3129,13 +3126,13 @@
     </row>
     <row r="35" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B35" s="27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="4">
@@ -3145,7 +3142,7 @@
         <v>110</v>
       </c>
       <c r="H35" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>23</v>
@@ -3158,7 +3155,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
@@ -3166,13 +3163,13 @@
     </row>
     <row r="36" spans="2:16" ht="48" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="4">
@@ -3182,13 +3179,13 @@
         <v>104</v>
       </c>
       <c r="H36" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K36" s="4">
         <v>4</v>
@@ -3197,23 +3194,23 @@
         <v>1</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
     </row>
     <row r="37" spans="2:16" ht="36" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="4">
@@ -3223,13 +3220,13 @@
         <v>105</v>
       </c>
       <c r="H37" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K37" s="4">
         <v>3</v>
@@ -3238,23 +3235,23 @@
         <v>1</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
     <row r="38" spans="2:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="4">
@@ -3264,13 +3261,13 @@
         <v>193</v>
       </c>
       <c r="H38" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>192</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K38" s="4">
         <v>1</v>
@@ -3279,7 +3276,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
@@ -3287,13 +3284,13 @@
     </row>
     <row r="39" spans="2:16" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="4">
@@ -3303,7 +3300,7 @@
         <v>124</v>
       </c>
       <c r="H39" s="28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>76</v>
@@ -3315,8 +3312,8 @@
       <c r="L39" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M39" s="30" t="s">
-        <v>337</v>
+      <c r="M39" s="5" t="s">
+        <v>336</v>
       </c>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
@@ -3324,13 +3321,13 @@
     </row>
     <row r="40" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="4">
@@ -3340,7 +3337,7 @@
         <v>123</v>
       </c>
       <c r="H40" s="28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>50</v>
@@ -3351,7 +3348,7 @@
       </c>
       <c r="L40" s="15"/>
       <c r="M40" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
@@ -3359,13 +3356,13 @@
     </row>
     <row r="41" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E41" s="14"/>
       <c r="F41" s="4">
@@ -3375,13 +3372,13 @@
         <v>125</v>
       </c>
       <c r="H41" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>36</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K41" s="4">
         <v>1</v>
@@ -3390,7 +3387,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
@@ -3398,13 +3395,13 @@
     </row>
     <row r="42" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="4">
@@ -3414,7 +3411,7 @@
         <v>136</v>
       </c>
       <c r="H42" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>53</v>
@@ -3427,7 +3424,7 @@
         <v>12</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
@@ -3435,7 +3432,7 @@
     </row>
     <row r="43" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>101</v>
@@ -3451,10 +3448,10 @@
         <v>191</v>
       </c>
       <c r="H43" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J43" s="5"/>
       <c r="K43" s="4">
@@ -3464,7 +3461,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
@@ -3472,13 +3469,13 @@
     </row>
     <row r="44" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>212</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E44" s="14"/>
       <c r="F44" s="4">
@@ -3488,7 +3485,7 @@
         <v>182</v>
       </c>
       <c r="H44" s="28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I44" s="5" t="s">
         <v>87</v>
@@ -3500,8 +3497,8 @@
       <c r="L44" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M44" s="30" t="s">
-        <v>325</v>
+      <c r="M44" s="5" t="s">
+        <v>324</v>
       </c>
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
@@ -3509,13 +3506,13 @@
     </row>
     <row r="45" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>212</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E45" s="14"/>
       <c r="F45" s="4">
@@ -3525,7 +3522,7 @@
         <v>186</v>
       </c>
       <c r="H45" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>92</v>
@@ -3537,8 +3534,8 @@
       <c r="L45" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="M45" s="30" t="s">
-        <v>326</v>
+      <c r="M45" s="5" t="s">
+        <v>325</v>
       </c>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
@@ -3546,13 +3543,13 @@
     </row>
     <row r="46" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>212</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="4">
@@ -3562,7 +3559,7 @@
         <v>199</v>
       </c>
       <c r="H46" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>89</v>
@@ -3574,8 +3571,8 @@
       <c r="L46" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="M46" s="30" t="s">
-        <v>320</v>
+      <c r="M46" s="5" t="s">
+        <v>319</v>
       </c>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
@@ -3583,13 +3580,13 @@
     </row>
     <row r="47" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>212</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="4">
@@ -3599,7 +3596,7 @@
         <v>184</v>
       </c>
       <c r="H47" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>90</v>
@@ -3611,8 +3608,8 @@
       <c r="L47" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="M47" s="30" t="s">
-        <v>321</v>
+      <c r="M47" s="5" t="s">
+        <v>320</v>
       </c>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
@@ -3620,13 +3617,13 @@
     </row>
     <row r="48" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>212</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="4">
@@ -3636,13 +3633,13 @@
         <v>198</v>
       </c>
       <c r="H48" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>197</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K48" s="4">
         <v>1</v>
@@ -3650,8 +3647,8 @@
       <c r="L48" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="M48" s="30" t="s">
-        <v>322</v>
+      <c r="M48" s="5" t="s">
+        <v>321</v>
       </c>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
@@ -3659,13 +3656,13 @@
     </row>
     <row r="49" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>212</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="4">
@@ -3675,7 +3672,7 @@
         <v>183</v>
       </c>
       <c r="H49" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>88</v>
@@ -3687,8 +3684,8 @@
       <c r="L49" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M49" s="30" t="s">
-        <v>327</v>
+      <c r="M49" s="5" t="s">
+        <v>326</v>
       </c>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
@@ -3696,13 +3693,13 @@
     </row>
     <row r="50" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>212</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="4">
@@ -3712,7 +3709,7 @@
         <v>185</v>
       </c>
       <c r="H50" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>91</v>
@@ -3724,8 +3721,8 @@
       <c r="L50" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="M50" s="30" t="s">
-        <v>323</v>
+      <c r="M50" s="5" t="s">
+        <v>322</v>
       </c>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
@@ -3733,13 +3730,13 @@
     </row>
     <row r="51" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E51" s="14"/>
       <c r="F51" s="4">
@@ -3749,13 +3746,13 @@
         <v>126</v>
       </c>
       <c r="H51" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>37</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K51" s="4">
         <v>1</v>
@@ -3764,7 +3761,7 @@
         <v>0</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
@@ -3772,13 +3769,13 @@
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E52" s="14"/>
       <c r="F52" s="4">
@@ -3788,7 +3785,7 @@
         <v>128</v>
       </c>
       <c r="H52" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>39</v>
@@ -3801,7 +3798,7 @@
         <v>2</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
@@ -3809,13 +3806,13 @@
     </row>
     <row r="53" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B53" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E53" s="14"/>
       <c r="F53" s="4">
@@ -3825,13 +3822,13 @@
         <v>129</v>
       </c>
       <c r="H53" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>40</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K53" s="4">
         <v>1</v>
@@ -3840,7 +3837,7 @@
         <v>3</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
@@ -3848,13 +3845,13 @@
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="4">
@@ -3864,7 +3861,7 @@
         <v>127</v>
       </c>
       <c r="H54" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>38</v>
@@ -3877,7 +3874,7 @@
         <v>1</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N54" s="5"/>
       <c r="O54" s="5"/>
@@ -3885,13 +3882,13 @@
     </row>
     <row r="55" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>208</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E55" s="14"/>
       <c r="F55" s="4">
@@ -3901,13 +3898,13 @@
         <v>130</v>
       </c>
       <c r="H55" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>41</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K55" s="4">
         <v>1</v>
@@ -3915,8 +3912,8 @@
       <c r="L55" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="M55" s="30" t="s">
-        <v>324</v>
+      <c r="M55" s="5" t="s">
+        <v>323</v>
       </c>
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
@@ -3924,13 +3921,13 @@
     </row>
     <row r="56" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E56" s="14"/>
       <c r="F56" s="4">
@@ -3940,10 +3937,10 @@
         <v>132</v>
       </c>
       <c r="H56" s="28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="4">
@@ -3952,8 +3949,8 @@
       <c r="L56" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M56" s="30" t="s">
-        <v>328</v>
+      <c r="M56" s="5" t="s">
+        <v>327</v>
       </c>
       <c r="N56" s="5"/>
       <c r="O56" s="5"/>
@@ -3961,13 +3958,13 @@
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B57" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>208</v>
       </c>
       <c r="D57" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E57" s="14"/>
       <c r="F57" s="4">
@@ -3977,7 +3974,7 @@
         <v>131</v>
       </c>
       <c r="H57" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>42</v>
@@ -3989,8 +3986,8 @@
       <c r="L57" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="M57" s="30" t="s">
-        <v>329</v>
+      <c r="M57" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="N57" s="5"/>
       <c r="O57" s="5"/>
@@ -3998,23 +3995,23 @@
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>208</v>
       </c>
       <c r="D58" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E58" s="14"/>
       <c r="F58" s="4">
         <v>14</v>
       </c>
-      <c r="G58" s="5" t="s">
+      <c r="G58" s="22" t="s">
         <v>133</v>
       </c>
       <c r="H58" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>44</v>
@@ -4026,8 +4023,8 @@
       <c r="L58" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="M58" s="30" t="s">
-        <v>330</v>
+      <c r="M58" s="5" t="s">
+        <v>329</v>
       </c>
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
@@ -4035,13 +4032,13 @@
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>204</v>
       </c>
       <c r="D59" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E59" s="14"/>
       <c r="F59" s="4">
@@ -4051,7 +4048,7 @@
         <v>113</v>
       </c>
       <c r="H59" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>24</v>
@@ -4063,8 +4060,8 @@
       <c r="L59" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="M59" s="30" t="s">
-        <v>331</v>
+      <c r="M59" s="5" t="s">
+        <v>330</v>
       </c>
       <c r="N59" s="5"/>
       <c r="O59" s="5"/>
@@ -4072,7 +4069,7 @@
     </row>
     <row r="60" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>99</v>
@@ -4103,7 +4100,7 @@
     </row>
     <row r="61" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>99</v>
@@ -4134,7 +4131,7 @@
     </row>
     <row r="62" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>99</v>
@@ -4165,7 +4162,7 @@
     </row>
     <row r="63" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>99</v>
@@ -4196,7 +4193,7 @@
     </row>
     <row r="64" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>99</v>
@@ -4227,7 +4224,7 @@
     </row>
     <row r="65" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>99</v>
@@ -4256,7 +4253,7 @@
     </row>
     <row r="66" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>99</v>
@@ -4287,7 +4284,7 @@
     </row>
     <row r="67" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>99</v>
@@ -4318,13 +4315,13 @@
     </row>
     <row r="68" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B68" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>204</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E68" s="14"/>
       <c r="F68" s="4">
@@ -4334,7 +4331,7 @@
         <v>114</v>
       </c>
       <c r="H68" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>25</v>
@@ -4346,8 +4343,8 @@
       <c r="L68" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="M68" s="30" t="s">
-        <v>332</v>
+      <c r="M68" s="5" t="s">
+        <v>331</v>
       </c>
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
@@ -4355,13 +4352,13 @@
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B69" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>211</v>
       </c>
       <c r="D69" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E69" s="14"/>
       <c r="F69" s="4">
@@ -4371,7 +4368,7 @@
         <v>189</v>
       </c>
       <c r="H69" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>95</v>
@@ -4383,8 +4380,8 @@
       <c r="L69" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="M69" s="30" t="s">
-        <v>333</v>
+      <c r="M69" s="5" t="s">
+        <v>332</v>
       </c>
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
@@ -4392,7 +4389,7 @@
     </row>
     <row r="70" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>209</v>
@@ -4417,7 +4414,7 @@
         <v>2</v>
       </c>
       <c r="M70" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N70" s="5"/>
       <c r="O70" s="5"/>
@@ -4425,7 +4422,7 @@
     </row>
     <row r="71" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>209</v>
@@ -4450,7 +4447,7 @@
         <v>2</v>
       </c>
       <c r="M71" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N71" s="5"/>
       <c r="O71" s="5"/>
@@ -4458,7 +4455,7 @@
     </row>
     <row r="72" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>209</v>
@@ -4489,7 +4486,7 @@
     </row>
     <row r="73" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>209</v>
@@ -4520,7 +4517,7 @@
     </row>
     <row r="74" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>209</v>
@@ -4545,7 +4542,7 @@
         <v>0</v>
       </c>
       <c r="M74" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N74" s="5"/>
       <c r="O74" s="5"/>
@@ -4553,7 +4550,7 @@
     </row>
     <row r="75" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>209</v>
@@ -4578,7 +4575,7 @@
         <v>0</v>
       </c>
       <c r="M75" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N75" s="5"/>
       <c r="O75" s="5"/>
@@ -4586,7 +4583,7 @@
     </row>
     <row r="76" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>209</v>
@@ -4611,7 +4608,7 @@
         <v>0</v>
       </c>
       <c r="M76" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N76" s="5"/>
       <c r="O76" s="5"/>
@@ -4619,7 +4616,7 @@
     </row>
     <row r="77" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>209</v>
@@ -4650,7 +4647,7 @@
     </row>
     <row r="78" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>209</v>
@@ -4681,7 +4678,7 @@
     </row>
     <row r="79" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>209</v>
@@ -4706,7 +4703,7 @@
         <v>3</v>
       </c>
       <c r="M79" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N79" s="5"/>
       <c r="O79" s="5"/>
@@ -4714,7 +4711,7 @@
     </row>
     <row r="80" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>209</v>
@@ -4739,7 +4736,7 @@
         <v>3</v>
       </c>
       <c r="M80" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N80" s="5"/>
       <c r="O80" s="5"/>
@@ -4747,7 +4744,7 @@
     </row>
     <row r="81" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>209</v>
@@ -4772,7 +4769,7 @@
         <v>3</v>
       </c>
       <c r="M81" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N81" s="5"/>
       <c r="O81" s="5"/>
@@ -4780,7 +4777,7 @@
     </row>
     <row r="82" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>209</v>
@@ -4811,7 +4808,7 @@
     </row>
     <row r="83" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>209</v>
@@ -4842,7 +4839,7 @@
     </row>
     <row r="84" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B84" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>209</v>
@@ -4867,7 +4864,7 @@
         <v>3</v>
       </c>
       <c r="M84" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N84" s="5"/>
       <c r="O84" s="5"/>
@@ -4875,7 +4872,7 @@
     </row>
     <row r="85" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>209</v>
@@ -4900,7 +4897,7 @@
         <v>1</v>
       </c>
       <c r="M85" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N85" s="5"/>
       <c r="O85" s="5"/>
@@ -4908,7 +4905,7 @@
     </row>
     <row r="86" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>209</v>
@@ -4933,7 +4930,7 @@
         <v>1</v>
       </c>
       <c r="M86" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N86" s="5"/>
       <c r="O86" s="5"/>
@@ -4941,7 +4938,7 @@
     </row>
     <row r="87" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>209</v>
@@ -4972,13 +4969,13 @@
     </row>
     <row r="88" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B88" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>211</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E88" s="14"/>
       <c r="F88" s="4">
@@ -4988,7 +4985,7 @@
         <v>187</v>
       </c>
       <c r="H88" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I88" s="5" t="s">
         <v>94</v>
@@ -5000,8 +4997,8 @@
       <c r="L88" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="M88" s="30" t="s">
-        <v>334</v>
+      <c r="M88" s="5" t="s">
+        <v>333</v>
       </c>
       <c r="N88" s="5"/>
       <c r="O88" s="5"/>
@@ -5009,13 +5006,13 @@
     </row>
     <row r="89" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B89" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>211</v>
       </c>
       <c r="D89" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E89" s="14"/>
       <c r="F89" s="4">
@@ -5025,7 +5022,7 @@
         <v>190</v>
       </c>
       <c r="H89" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I89" s="5" t="s">
         <v>97</v>
@@ -5037,8 +5034,8 @@
       <c r="L89" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M89" s="30" t="s">
-        <v>335</v>
+      <c r="M89" s="5" t="s">
+        <v>334</v>
       </c>
       <c r="N89" s="5"/>
       <c r="O89" s="5"/>
@@ -5046,13 +5043,13 @@
     </row>
     <row r="90" spans="2:16" ht="24" x14ac:dyDescent="0.25">
       <c r="B90" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>211</v>
       </c>
       <c r="D90" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E90" s="14"/>
       <c r="F90" s="4">
@@ -5062,7 +5059,7 @@
         <v>188</v>
       </c>
       <c r="H90" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I90" s="5" t="s">
         <v>96</v>
@@ -5074,8 +5071,8 @@
       <c r="L90" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="M90" s="30" t="s">
-        <v>336</v>
+      <c r="M90" s="5" t="s">
+        <v>335</v>
       </c>
       <c r="N90" s="5"/>
       <c r="O90" s="5"/>
@@ -5083,13 +5080,13 @@
     </row>
     <row r="91" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B91" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D91" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E91" s="14"/>
       <c r="F91" s="4">
@@ -5099,13 +5096,13 @@
         <v>122</v>
       </c>
       <c r="H91" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I91" s="5" t="s">
         <v>48</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K91" s="4">
         <v>1</v>
@@ -5114,7 +5111,7 @@
         <v>1</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N91" s="5"/>
       <c r="O91" s="5"/>
@@ -5122,13 +5119,13 @@
     </row>
     <row r="92" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B92" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D92" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E92" s="14"/>
       <c r="F92" s="4">
@@ -5138,13 +5135,13 @@
         <v>121</v>
       </c>
       <c r="H92" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I92" s="5" t="s">
         <v>47</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K92" s="4">
         <v>1</v>
@@ -5153,7 +5150,7 @@
         <v>10</v>
       </c>
       <c r="M92" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N92" s="5"/>
       <c r="O92" s="5"/>
@@ -5161,29 +5158,29 @@
     </row>
     <row r="93" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B93" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>205</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E93" s="14"/>
       <c r="F93" s="4">
         <v>30</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>214</v>
+        <v>337</v>
       </c>
       <c r="H93" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I93" s="5" t="s">
         <v>194</v>
       </c>
       <c r="J93" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K93" s="4">
         <v>1</v>
@@ -5192,7 +5189,7 @@
         <v>3</v>
       </c>
       <c r="M93" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N93" s="5"/>
       <c r="O93" s="5"/>
@@ -5200,7 +5197,7 @@
     </row>
     <row r="94" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B94" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>210</v>
@@ -5231,7 +5228,7 @@
     </row>
     <row r="95" spans="2:16" ht="24" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>210</v>
@@ -5262,7 +5259,7 @@
     </row>
     <row r="96" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B96" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>210</v>
@@ -5293,7 +5290,7 @@
     </row>
     <row r="97" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B97" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>210</v>
@@ -5324,7 +5321,7 @@
     </row>
     <row r="98" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B98" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>210</v>
@@ -5355,7 +5352,7 @@
     </row>
     <row r="99" spans="2:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B99" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>210</v>

</xml_diff>

<commit_message>
Cumulative update of 25 Apr 2025 (see rel. notes)
</commit_message>
<xml_diff>
--- a/iApply_CCBS_Interfaces.xlsx
+++ b/iApply_CCBS_Interfaces.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B210854F-520D-4F4C-9939-AC4B82AB1207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B532576-8C83-448D-B2C8-26307F6FDA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="429" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CCBS_API_CALLS" sheetId="5" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="345">
   <si>
     <t>INSERT</t>
   </si>
@@ -1131,6 +1131,9 @@
   </si>
   <si>
     <t>Order sequence:</t>
+  </si>
+  <si>
+    <t>Properties</t>
   </si>
 </sst>
 </file>
@@ -2024,8 +2027,8 @@
   <dimension ref="A1:T101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="2" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -2033,7 +2036,7 @@
     <col min="1" max="1" width="1.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" style="16" customWidth="1"/>
     <col min="5" max="5" width="15.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2209,7 +2212,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
         <v>268</v>
@@ -2571,7 +2574,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="2:17" ht="36" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:17" ht="48" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
         <v>268</v>
@@ -2611,7 +2614,7 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
     </row>
-    <row r="15" spans="2:17" ht="36" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
         <v>268</v>
@@ -2689,7 +2692,7 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
     </row>
-    <row r="17" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17" s="27">
         <v>45505</v>
       </c>
@@ -2799,7 +2802,7 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
         <v>268</v>
@@ -2875,7 +2878,7 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="1:17" ht="48" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
         <v>268</v>
@@ -2915,7 +2918,7 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
     </row>
-    <row r="23" spans="1:17" ht="36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
         <v>268</v>
@@ -2953,7 +2956,7 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
     </row>
-    <row r="24" spans="1:17" ht="48" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
         <v>268</v>
@@ -3110,7 +3113,7 @@
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
     </row>
-    <row r="28" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
         <v>268</v>
@@ -3148,7 +3151,7 @@
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
     </row>
-    <row r="29" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="36" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
         <v>268</v>
@@ -3190,7 +3193,7 @@
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
     </row>
-    <row r="30" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="36" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5" t="s">
         <v>268</v>
@@ -3384,7 +3387,7 @@
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
     </row>
-    <row r="35" spans="2:17" s="25" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
         <v>268</v>
@@ -3462,7 +3465,7 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
     </row>
-    <row r="37" spans="2:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:17" ht="48" x14ac:dyDescent="0.3">
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
         <v>268</v>
@@ -3504,7 +3507,7 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
     </row>
-    <row r="38" spans="2:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:17" ht="36" x14ac:dyDescent="0.3">
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
         <v>268</v>
@@ -3586,7 +3589,7 @@
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
     </row>
-    <row r="40" spans="2:17" ht="36" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:17" ht="24" x14ac:dyDescent="0.3">
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
         <v>268</v>
@@ -3820,7 +3823,7 @@
       <c r="P45" s="4"/>
       <c r="Q45" s="4"/>
     </row>
-    <row r="46" spans="2:17" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:17" ht="24" x14ac:dyDescent="0.3">
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
         <v>268</v>
@@ -3894,7 +3897,7 @@
       <c r="P47" s="4"/>
       <c r="Q47" s="4"/>
     </row>
-    <row r="48" spans="2:17" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
         <v>268</v>
@@ -4492,7 +4495,7 @@
       <c r="P64" s="4"/>
       <c r="Q64" s="4"/>
     </row>
-    <row r="65" spans="2:17" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="8"/>
       <c r="C65" s="8" t="s">
         <v>270</v>
@@ -4524,7 +4527,7 @@
       <c r="P65" s="4"/>
       <c r="Q65" s="4"/>
     </row>
-    <row r="66" spans="2:17" ht="36" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" ht="36" x14ac:dyDescent="0.3">
       <c r="B66" s="8"/>
       <c r="C66" s="8" t="s">
         <v>270</v>
@@ -4556,7 +4559,7 @@
       <c r="P66" s="4"/>
       <c r="Q66" s="4"/>
     </row>
-    <row r="67" spans="2:17" ht="36" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" ht="36" x14ac:dyDescent="0.3">
       <c r="B67" s="8"/>
       <c r="C67" s="8" t="s">
         <v>270</v>
@@ -4588,7 +4591,7 @@
       <c r="P67" s="4"/>
       <c r="Q67" s="4"/>
     </row>
-    <row r="68" spans="2:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="8"/>
       <c r="C68" s="8" t="s">
         <v>270</v>
@@ -4620,7 +4623,7 @@
       <c r="P68" s="4"/>
       <c r="Q68" s="4"/>
     </row>
-    <row r="69" spans="2:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="8"/>
       <c r="C69" s="8" t="s">
         <v>270</v>
@@ -4652,7 +4655,7 @@
       <c r="P69" s="4"/>
       <c r="Q69" s="4"/>
     </row>
-    <row r="70" spans="2:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="8"/>
       <c r="C70" s="8" t="s">
         <v>270</v>
@@ -4684,7 +4687,7 @@
       <c r="P70" s="4"/>
       <c r="Q70" s="4"/>
     </row>
-    <row r="71" spans="2:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="B71" s="8"/>
       <c r="C71" s="8" t="s">
         <v>270</v>
@@ -4716,7 +4719,7 @@
       <c r="P71" s="4"/>
       <c r="Q71" s="4"/>
     </row>
-    <row r="72" spans="2:17" ht="36" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" ht="36" x14ac:dyDescent="0.3">
       <c r="B72" s="8"/>
       <c r="C72" s="8" t="s">
         <v>270</v>
@@ -4748,7 +4751,7 @@
       <c r="P72" s="4"/>
       <c r="Q72" s="4"/>
     </row>
-    <row r="73" spans="2:17" ht="36" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" ht="36" x14ac:dyDescent="0.3">
       <c r="B73" s="8"/>
       <c r="C73" s="8" t="s">
         <v>270</v>
@@ -4780,7 +4783,7 @@
       <c r="P73" s="4"/>
       <c r="Q73" s="4"/>
     </row>
-    <row r="74" spans="2:17" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="8"/>
       <c r="C74" s="8" t="s">
         <v>270</v>
@@ -4812,15 +4815,18 @@
       <c r="P74" s="4"/>
       <c r="Q74" s="4"/>
     </row>
-    <row r="75" spans="2:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+      <c r="A75" s="28"/>
       <c r="B75" s="8"/>
-      <c r="C75" s="8" t="s">
-        <v>270</v>
+      <c r="C75" s="6" t="s">
+        <v>269</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="E75" s="18"/>
+      <c r="E75" s="18" t="s">
+        <v>344</v>
+      </c>
       <c r="F75" s="4"/>
       <c r="G75" s="3">
         <v>999</v>
@@ -4846,7 +4852,7 @@
       <c r="P75" s="4"/>
       <c r="Q75" s="4"/>
     </row>
-    <row r="76" spans="2:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="B76" s="8"/>
       <c r="C76" s="8" t="s">
         <v>270</v>
@@ -4880,7 +4886,7 @@
       <c r="P76" s="4"/>
       <c r="Q76" s="4"/>
     </row>
-    <row r="77" spans="2:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="B77" s="8"/>
       <c r="C77" s="8" t="s">
         <v>270</v>
@@ -4914,7 +4920,7 @@
       <c r="P77" s="4"/>
       <c r="Q77" s="4"/>
     </row>
-    <row r="78" spans="2:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="B78" s="8"/>
       <c r="C78" s="8" t="s">
         <v>270</v>
@@ -4946,7 +4952,7 @@
       <c r="P78" s="4"/>
       <c r="Q78" s="4"/>
     </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B79" s="8"/>
       <c r="C79" s="8" t="s">
         <v>270</v>
@@ -4978,7 +4984,7 @@
       <c r="P79" s="4"/>
       <c r="Q79" s="4"/>
     </row>
-    <row r="80" spans="2:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="B80" s="8"/>
       <c r="C80" s="8" t="s">
         <v>270</v>
@@ -5138,7 +5144,7 @@
       <c r="P84" s="4"/>
       <c r="Q84" s="4"/>
     </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:17" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="8"/>
       <c r="C85" s="8" t="s">
         <v>270</v>

</xml_diff>